<commit_message>
Bug List: Update the documents of Bug List. These files describe some defectives in the Linux Distributions running on the Xen as VMs.
sign-off-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\15.项目\03.UVP&amp;EVS V2R2C00 XEN 5.1U2\500.翻译稿\02. 开源UVP Tools相关文档\buglist\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="15390" windowHeight="7890" activeTab="2"/>
   </bookViews>
@@ -33,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="153">
   <si>
     <t>http://www.huawei.com</t>
   </si>
@@ -231,36 +226,16 @@
     <t>https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/diff/drivers/xen/xenbus/xenbus_dev_frontend.c?id=2fb3683e7b164ee2b324039f7c9d90fe5b1a259b</t>
   </si>
   <si>
-    <t xml:space="preserve">Domain0 fails to obtain in-band information about the VM. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">A VM does not provide an interface (such as the /proc/xen/xenbus or /dev/xen/xenbus file) for user-space programs to access xenbus. As a result, the uvp-monitor process fails to be run. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CentOS 6.5 and 6.6 (64-bit)
-Red Hat Enterprise Linux 6.6 (64-bit)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/drivers/net/xen-netfront.c?id=cefe0078eea52af17411eb1248946a94afb84ca5</t>
   </si>
   <si>
     <t xml:space="preserve">If the NIC of the VM has been hot-plugged for about 200 times, the VM no longer issues hot-plug commands against the NIC or a disk. </t>
   </si>
   <si>
-    <t>The Xen front-end NIC driver is defective. Resource leak occurs when a VM deletes the granted references.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=dd9d3843755da95f63dd3a376f62b3e45c011210</t>
   </si>
   <si>
     <t>The VM may fail to start up.</t>
-  </si>
-  <si>
-    <t>If a VM attempts to start up while the host CPU usage is high, the AP CPU may be scheduled to execute other tasks when its state is changing from online to active. In this case, if the boot CPU tries to migrate the kernel threads (for example, migration, ksoftirq, and watchdog threads) related to the hotplug thread of the AP CPU, the migration fails and these threads encounter a bug-on error.</t>
   </si>
   <si>
     <t>Fedora 22</t>
@@ -294,9 +269,6 @@
   </si>
   <si>
     <t xml:space="preserve">The VM kernel is defective. When a user-space program uses the /proc/xen/xenbus file to set a watch, the new FMODE_ATOMIC_POS added to the process file system of Linux kernel causes the program to encounter a deadlock on the RCU read lock. </t>
-  </si>
-  <si>
-    <t>openSUSE 13.2</t>
   </si>
   <si>
     <t>https://sourceware.org/git/gitweb.cgi?p=systemtap.git;a=commit;h=f2b610b6295628ae1fef744421c293883f1e4298</t>
@@ -375,23 +347,9 @@
     <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=c275a57f5ec3056f732843b11659d892235faff7</t>
   </si>
   <si>
-    <t xml:space="preserve">The actual free memory of the VM is smaller than the memory allocated by Xen hypervisor, and the VM sometimes crashes. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>When a VM calculates its maximum free memory, it counts the MMIO hole in. Therefore, the calculated free memory is greater than the actual free memory of the VM, triggering a balloon-out of the VM memory.</t>
   </si>
   <si>
-    <t>CentOS 6.5 (64-bit), 7.0, and 7.1
-Debian GNU and Linux 7.1.0 (32-bit and 64-bit)
-Novell SuSE Linux Enterprise Server 11 SP4 (64-bit)
-Novell SuSE Linux Enterprise Server 12 SP1 (64-bit)
-Oracle Linux 6.4 (32-bit and 64-bit)
-Red Hat Enterprise Linux 6.6, 7.0, and 7.1 (64-bit)
-Ubuntu 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=6a1f513776b78c994045287073e55bae44ed9f8c</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -403,13 +361,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CentOS 6.5 (64-bit)
-Debian 6, 7, and 8
-Versions 6.6, 6.7, and 7 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux
-Ubuntu 12, 13, 14, and 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Install the corrective patch or upgrade the kernel to version 2.6.32-504.12.2 or later.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -428,9 +379,6 @@
   </si>
   <si>
     <t xml:space="preserve">Upgrade the kernel to version 2.6.32-358.23.2 or later. </t>
-  </si>
-  <si>
-    <t>Contact OS vendors to obtain the corrective patch.</t>
   </si>
   <si>
     <t xml:space="preserve">After the live migration, the VM remains unresponsive for more than 15 minutes. During the VM downtime, operations on the VM are not allowed, including snapshot restoration, hibernation, and wake-up. </t>
@@ -462,10 +410,6 @@
 https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=cbb330045e5df8f665ac60227ff898421fc8fb92</t>
   </si>
   <si>
-    <t xml:space="preserve">The live migration, snapshot, or hibernation of the VM that uses Linux kernel 2.6.32 fails occasionally. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">The USB subsystem of Linux kernel 2.6.32 may fail to be suspended, forcibly terminating the VM suspend procedure. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -482,10 +426,6 @@
   </si>
   <si>
     <t xml:space="preserve">The default version of the xorg-x11-drv-cirrus component does not work well on the Xen. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Versions 6.4 and 6.5 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux (64-bit)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -498,33 +438,249 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>After a live VM migration, the VM is not pingable for about 10s and ping packets are discarded.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No official corrective patch is available. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">None. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red Hat Enterprise Linux 6.4 (32-bit)
+Versions 6.4 and 6.5 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux (64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CentOS 6.4, 6.5, and 6.7 (64-bit)
+Debian 6, 7, and 8
+Red Hat Enterprise Linux 6.4 (32-bit and 64-bit)
+Versions 6.6, 6.7, and 7 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux
+Ubuntu 12, 13, 14, and 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CentOS 5.11 (32-bit and 64-bit)
+CentOS 6.3, 6.4, 6.5, and 6.7 (64-bit)
+CentOS 6.6 (32-bit)
+Debian GNU and Linux 7.1.0 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 11 SP4 (64-bit)
+Oracle Linux 6.4 (32-bit and 64-bit)
+Oracle Linux 6.7 (64-bit)
+Red Hat Enterprise Linux 6.4 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.6, 7.0, and 7.1 (64-bit)
+Ubuntu 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.7 (64-bit)
+openSUSE 13.2 (64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.3, 6.4, 6.5, 6.7, and 7.0 (64-bit) 
+CentOS 6.6 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.4 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 6.6 (64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.3, 6.4, 6.5, and 6.7 (64-bit) 
+CentOS 6.6 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.4 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 6.6 (64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">During the VM restoration (after a VM is live migrated to the destination), the VM kernel restores the status of the Qemu-emulated device. This restoration operation lasts about 10s, during which, the VM fails to respond to network transmission requests. 
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>After a live VM migration, the VM is not pingable for about 10s and ping packets are discarded.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">No official corrective patch is available. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">None. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CentOS 6.5, 6.6 and 7.0 (64-bit)
-Red Hat Enterprise Linux 6.6 (64-bit)</t>
+    <t xml:space="preserve">The live migration, snapshot, or hibernation of the VM that uses Linux kernel 2.6.32 fails occasionally. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If a VM attempts to start up while the host CPU usage is high, the AP CPU may be scheduled to execute other tasks when its state is changing from online to active. In this case, if the boot CPU tries to migrate the kernel threads (for example, migration, ksoftirq, and watchdog threads) related to the hotplug thread of the AP CPU, the migration fails and these threads encounter a bug-on error.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Xen front-end NIC driver is defective. Resource leak occurs when a VM deletes the granted references.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. The balloon driver of the VM kernel incorrectly counts the IO configuration space and MMIO holes in when calculating the available memory size, so the calculated memory size is larger than the configured one. If the calculated memory size is larger than 4 GB, the VM performs memory balloon-out after it is started, causing the actual memory size of the VM to be smaller than the configured one. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The actual memory size displayed to users is smaller than the configured one. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network connectivity to the VM is abnormal. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective, causing uvp-monitor unable to be installed on the VM. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain0 fails to obtain the in-band information about the VM. </t>
+  </si>
+  <si>
+    <t>Oracle Linux 6.7 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. The VM sometimes stops responding if live migration is performed constantly. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the case of constant live migration, the VM may fail to respond after it is live migrated to the destination. </t>
+  </si>
+  <si>
+    <t>CentOS 5.11 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t>CentOS 6.3 (64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The virtual disk of a VM is unable to handle VM suspension failures. If the VM fails to be suspended, the granted references of the virtual disk are not released. In this case, resuming the virtual disk causes a failure in applying for granted references. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 12 (64-bit)
+Novell SuSE Linux Enterprise Server 12 SP1 (64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM does not respond when it is being restored using a snapshot. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bugzilla.redhat.com/show_bug.cgi?id=224662 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install the corrective patch to reduce the possibility of this problem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A VM does not provide an interface (such as the /proc/xen/xenbus or /dev/xen/xenbus file) for user-space programs to access xenbus. As a result, the uvp-monitor process fails to be run. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain0 fails to obtain in-band information about the VM. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>CentOS 5.11 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF010000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">32-bit and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>64-bit)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The "HWADDR=xx:xx:xx:xx" configuration option is missing in the VM NIC configuration file ifcfg-ethX. After the VM is restarted, the NIC fails to determine its name based on the MAC address in the ifcfg-ethX file. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">After the VM is restarted, the NIC name is changed to "_tmpx". </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Add the "HWADDR=xx:xx:xx:xx" configuration option to the /etc/sysconfig/network-scripts/ifcfg-ethX file. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contact OS vendors to obtain the corrective patch.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The actual free memory of the VM is smaller than the memory allocated by Xen hypervisor, and the VM sometimes crashes. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Log in to the VM, and run the lsmod | grep xen command to check whether the VM is armed with the Xen front-end driver. If "xen_vnif", "xen_vbd", and "xen_platform_pci" are displayed in the command output, the VM is armed with the Xen front-end driver. If the VM is not armed with the Xen front-end driver, do not use this VM any more. 
+2. Run the fdisk -l command to check whether the VM has two disk devices /dev/xvda and /dev/sda. Run the ifconfig –a command to check whether the VM has two NICs with identical MAC addresses. 
+3. If there are two disk devices on the VM, add "ide0=noprobe hdc=noprobe" to the /boot/grub/menu.lst file to disable the IDE disk. 
+4. If there are two NICs on the VM, add the following configurations at the end of the /etc/modprobe.d/blacklist.conf file to disable the 8139 NIC. 
+alias 8139cp off
+install 8139cp :
+alias 8139too off
+install 8139too :
+5. Run the mkinitrd -f /boot/initrd-$(uname -r).img $(uname -r) --with=xen_vbd --with=xen_vnif command to add the Xen front-end driver to the initrd file. 
+6. Restart the VM.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=72978b2fe2f2cdf9f319c6c6dcdbe92b38de2be2
+http://git.kernel.org/cgit/linux/kernel/git/tip/tip.git/commit/?id=c4288334818c81c946acb23d2319881f58c3d497</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add the following configurations at the end of the /etc/modprobe.d/blacklist.conf file to disable the 8139 NIC during the VM startup: 
+alias 8139cp off
+install 8139cp :
+alias 8139too off
+install 8139too :
+2. Restart the VM for the new configurations to take effect. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. If the Xen Hypervisor issues a hibernation operation to a VM, the XenStore watch of the VM will be deregistered. However, the XenStore watch is unable to handle VM hibernation failures. That is, if the hibernation of the VM fails, the XenStore watch that is deregistered during the hibernation does not re-register with the kernel. As a result, the subsequent operations issued by the XenStore watch fail. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The following operations issued by the XenStore watch fail: 
+VM reboot 
+Live migration 
+Hibernation 
+Snapshot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The live migration, snapshot, or hibernation of the VM fails. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a VM uses the Qemu-emulated IDE disks instead of Xen paravirtual disks. During live migration, snapshot, or hibernation, the VM needs to be suspended. Once the VM is suspended, the Qemu on the VM is expected to stop, and the IO in the cache is expected to be updated to the Qemu-emulated IDE disks. However, the Qemu-emulated IDE disks are unable to handle the IO update. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM is defective. The VM is armed with two NICs whose MAC addresses are the same. One is the Qemu-emulated 8139 NIC; the other is the Xen paravirtual NIC. If these two NICs obtain IP addresses through DHCP, they may be assigned the same IP address. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="41">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="42">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,12 +920,6 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -786,6 +936,19 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF010000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -865,7 +1028,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -974,24 +1137,60 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1017,19 +1216,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1211,7 +1398,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="MML命令目录"/>
@@ -1375,7 +1562,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1407,10 +1594,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1442,7 +1628,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1618,7 +1803,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -1638,71 +1823,71 @@
   <sheetData>
     <row r="1" spans="1:10" ht="35.1" customHeight="1">
       <c r="A1" s="3"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="55"/>
     </row>
     <row r="2" spans="1:10" ht="37.35" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="43"/>
+      <c r="E2" s="55"/>
     </row>
     <row r="3" spans="1:10" ht="259.35000000000002" customHeight="1">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="43"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="55"/>
     </row>
     <row r="4" spans="1:10" ht="111.6" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46" t="s">
+      <c r="A4" s="57"/>
+      <c r="B4" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="43"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="1:10" ht="18.600000000000001" customHeight="1">
-      <c r="A5" s="45"/>
+      <c r="A5" s="57"/>
       <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="43"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="55"/>
     </row>
     <row r="6" spans="1:10" ht="18.600000000000001" customHeight="1">
-      <c r="A6" s="45"/>
+      <c r="A6" s="57"/>
       <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="43"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="55"/>
     </row>
     <row r="7" spans="1:10" ht="130.35" customHeight="1">
-      <c r="A7" s="45"/>
-      <c r="B7" s="48" t="s">
+      <c r="A7" s="57"/>
+      <c r="B7" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="43"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A8" s="45"/>
+      <c r="A8" s="57"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="43"/>
+      <c r="E8" s="55"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -1710,21 +1895,21 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="33" customHeight="1">
-      <c r="A9" s="45"/>
+      <c r="A9" s="57"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="43"/>
+      <c r="E9" s="55"/>
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -1746,13 +1931,13 @@
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -1760,13 +1945,13 @@
       <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" ht="23.25" customHeight="1">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -1788,11 +1973,11 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -1800,13 +1985,13 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -1854,11 +2039,11 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" ht="20.25">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1885,11 +2070,11 @@
       <c r="A22" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="54"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
       <c r="E22" s="15"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1900,11 +2085,11 @@
       <c r="A23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -1931,14 +2116,6 @@
     <row r="38" ht="13.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:D22"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:E9"/>
@@ -1952,6 +2129,14 @@
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:D22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -1969,7 +2154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -1991,10 +2176,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" customHeight="1">
       <c r="A2" s="19"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="58"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:3" ht="46.5">
       <c r="A3" s="21" t="s">
@@ -2004,17 +2189,17 @@
     </row>
     <row r="4" spans="1:3" ht="114" customHeight="1">
       <c r="A4" s="19"/>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="66"/>
     </row>
     <row r="5" spans="1:3" ht="46.5">
       <c r="A5" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="22"/>
@@ -2023,55 +2208,55 @@
       <c r="A7" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="56"/>
+      <c r="C7" s="64"/>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1">
       <c r="A8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="56"/>
+      <c r="C8" s="64"/>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1">
       <c r="A9" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="56"/>
+      <c r="C9" s="64"/>
     </row>
     <row r="10" spans="1:3" ht="21" customHeight="1">
       <c r="A10" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="56"/>
+      <c r="C10" s="64"/>
     </row>
     <row r="11" spans="1:3" ht="34.5" customHeight="1">
       <c r="A11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="56"/>
+      <c r="C11" s="64"/>
     </row>
     <row r="12" spans="1:3" ht="31.5" customHeight="1">
       <c r="A12" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="57"/>
+      <c r="C12" s="65"/>
     </row>
     <row r="13" spans="1:3" ht="13.5" customHeight="1">
       <c r="A13" s="23"/>
@@ -2091,10 +2276,10 @@
     </row>
     <row r="16" spans="1:3" ht="34.5" customHeight="1">
       <c r="A16" s="19"/>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="55"/>
+      <c r="C16" s="63"/>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="25" t="s">
@@ -2152,81 +2337,81 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.375" customWidth="1"/>
     <col min="2" max="2" width="48" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5" customWidth="1"/>
+    <col min="3" max="3" width="47.5" customWidth="1"/>
     <col min="4" max="4" width="31.375" customWidth="1"/>
     <col min="5" max="5" width="61.5" style="31" customWidth="1"/>
-    <col min="6" max="6" width="55" customWidth="1"/>
+    <col min="6" max="6" width="57.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="42.75" customHeight="1">
-      <c r="A1" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="40" t="s">
+    <row r="1" spans="1:6" ht="15.75">
+      <c r="A1" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60" customHeight="1">
+    <row r="2" spans="1:6" ht="47.25">
       <c r="A2" s="32">
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>115</v>
+        <v>106</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>104</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="97.5" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="94.5">
       <c r="A3" s="32">
         <v>2</v>
       </c>
       <c r="B3" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>111</v>
-      </c>
       <c r="F3" s="32" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="78.75">
@@ -2234,19 +2419,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="94.5">
@@ -2254,19 +2439,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="47.25">
@@ -2274,136 +2459,136 @@
         <v>5</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="101.25" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="94.5">
       <c r="A7" s="32">
         <v>6</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>85</v>
       </c>
       <c r="F7" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="119.25" customHeight="1">
+    <row r="8" spans="1:6" ht="157.5">
       <c r="A8" s="32">
         <v>7</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F8" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="187.5" customHeight="1">
+    <row r="9" spans="1:6" ht="173.25">
       <c r="A9" s="32">
         <v>8</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="107.25" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="94.5">
       <c r="A10" s="32">
         <v>9</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="108" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="94.5">
       <c r="A11" s="32">
         <v>10</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="51.75" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="31.5">
       <c r="A12" s="32">
         <v>11</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D12" s="32" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>49</v>
@@ -2414,93 +2599,93 @@
         <v>12</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D13" s="32" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E13" s="33" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F13" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="130.5" customHeight="1">
+    <row r="14" spans="1:6" ht="110.25">
       <c r="A14" s="32">
         <v>13</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D14" s="32" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F14" s="32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="117.75" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="110.25">
       <c r="A15" s="32">
         <v>14</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="D15" s="32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E15" s="33" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F15" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="72.75" customHeight="1">
+    <row r="16" spans="1:6" ht="78.75">
       <c r="A16" s="32">
         <v>15</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F16" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="73.5" customHeight="1">
+    <row r="17" spans="1:6" ht="78.75">
       <c r="A17" s="32">
         <v>16</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="D17" s="32" t="s">
-        <v>51</v>
+        <v>138</v>
       </c>
       <c r="E17" s="33" t="s">
         <v>50</v>
@@ -2514,20 +2699,183 @@
         <v>17</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D18" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="126">
+      <c r="A19" s="40">
+        <v>18</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="D19" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="E19" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="126">
+      <c r="A20" s="42">
+        <v>19</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="40" t="s">
         <v>124</v>
       </c>
+      <c r="E20" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="31.5">
+      <c r="A21" s="44">
+        <v>20</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="63">
+      <c r="A22" s="44">
+        <v>21</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C22" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="63">
+      <c r="A23" s="44">
+        <v>22</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="315">
+      <c r="A24" s="44">
+        <v>23</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="126">
+      <c r="A25" s="44">
+        <v>24</v>
+      </c>
+      <c r="B25" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="78.75">
+      <c r="A26" s="44">
+        <v>25</v>
+      </c>
+      <c r="B26" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="B28" s="48"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2541,8 +2889,9 @@
     <hyperlink ref="E16" r:id="rId7"/>
     <hyperlink ref="E17" r:id="rId8"/>
     <hyperlink ref="E7" r:id="rId9"/>
+    <hyperlink ref="E22" r:id="rId10" display="https://bugzilla.redhat.com/show_bug.cgi?id=224662"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs/buglist: Update the buglist of Linux distributions as a VM.
Add CoreOS's defectives run as a VM on the xen.

Signed-off-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15390" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15600" windowHeight="10965"/>
   </bookViews>
   <sheets>
     <sheet name="About This Document" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <definedName name="_Hlt448738431" localSheetId="1">'Bug List'!$C$15</definedName>
     <definedName name="_Hlt448752930" localSheetId="1">'Bug List'!$F$12</definedName>
     <definedName name="_Hlt448771702" localSheetId="1">'Bug List'!$C$13</definedName>
+    <definedName name="_Hlt456345688" localSheetId="1">'Bug List'!$C$33</definedName>
     <definedName name="unitENG">[1]数据固化!$AB$4:$AB$21</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="149">
   <si>
     <t>Issue</t>
   </si>
@@ -201,11 +202,6 @@
   <si>
     <t xml:space="preserve">The VM kernel is defective. During VM live migration, the VM kernel performs suspend and resume operations on Xen devices (front-end and back-end) and Qemu-emulated device. The operations on the Qemu-emulated device take about 10 seconds, during which the VM fails to respond to external requests. </t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CentOS 6.5 (64-bit)
-Oracle Linux Server 6.3 to 6.5 (32-bit and 64-bit)
-Red Hat Enterprise Linux 6.6 (64-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">Upgrade the udev to 204-5ubuntu13 or later. </t>
@@ -357,71 +353,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Red Hat Enterprise Linux 6.4 (32-bit)
-Versions 6.4 and 6.5 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux (64-bit)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CentOS 6.4, 6.5, and 6.7 (64-bit)
-Debian 6, 7, and 8
-Red Hat Enterprise Linux 6.4 (32-bit and 64-bit)
-Versions 6.6, 6.7, and 7 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux
-Ubuntu 12, 13, 14, and 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CentOS 5.11 (32-bit and 64-bit)
-CentOS 6.3, 6.4, 6.5, and 6.7 (64-bit)
-CentOS 6.6 (32-bit)
-Debian GNU and Linux 7.1.0 (32-bit and 64-bit)
-Novell SuSE Linux Enterprise Server 11 SP4 (64-bit)
-Oracle Linux 6.4 (32-bit and 64-bit)
-Oracle Linux 6.7 (64-bit)
-Red Hat Enterprise Linux 6.4 (32-bit and 64-bit)
-Red Hat Enterprise Linux 6.6, 7.0, and 7.1 (64-bit)
-Ubuntu 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CentOS 6.7 (64-bit)
-openSUSE 13.2 (64-bit)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CentOS 6.3, 6.4, 6.5, 6.7, and 7.0 (64-bit) 
-CentOS 6.6 (32-bit and 64-bit)
-Red Hat Enterprise Linux 6.4 (32-bit and 64-bit) 
-Red Hat Enterprise Linux 6.6 (64-bit)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CentOS 6.3, 6.4, 6.5, and 6.7 (64-bit) 
-CentOS 6.6 (32-bit and 64-bit)
-Red Hat Enterprise Linux 6.4 (32-bit and 64-bit) 
-Red Hat Enterprise Linux 6.6 (64-bit)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">During the VM restoration (after a VM is live migrated to the destination), the VM kernel restores the status of the Qemu-emulated device. This restoration operation lasts about 10s, during which, the VM fails to respond to network transmission requests. 
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The live migration, snapshot, or hibernation of the VM that uses Linux kernel 2.6.32 fails occasionally. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>If a VM attempts to start up while the host CPU usage is high, the AP CPU may be scheduled to execute other tasks when its state is changing from online to active. In this case, if the boot CPU tries to migrate the kernel threads (for example, migration, ksoftirq, and watchdog threads) related to the hotplug thread of the AP CPU, the migration fails and these threads encounter a bug-on error.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Xen front-end NIC driver is defective. Resource leak occurs when a VM deletes the granted references.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">The VM kernel is defective. The balloon driver of the VM kernel incorrectly counts the IO configuration space and MMIO holes in when calculating the available memory size, so the calculated memory size is larger than the configured one. If the calculated memory size is larger than 4 GB, the VM performs memory balloon-out after it is started, causing the actual memory size of the VM to be smaller than the configured one. </t>
   </si>
   <si>
@@ -455,28 +386,10 @@
     <t xml:space="preserve">The virtual disk of a VM is unable to handle VM suspension failures. If the VM fails to be suspended, the granted references of the virtual disk are not released. In this case, resuming the virtual disk causes a failure in applying for granted references. </t>
   </si>
   <si>
-    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 12 (64-bit)
-Novell SuSE Linux Enterprise Server 12 SP1 (64-bit)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The VM does not respond when it is being restored using a snapshot. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">https://bugzilla.redhat.com/show_bug.cgi?id=224662 </t>
   </si>
   <si>
     <t xml:space="preserve">Install the corrective patch to reduce the possibility of this problem. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A VM does not provide an interface (such as the /proc/xen/xenbus or /dev/xen/xenbus file) for user-space programs to access xenbus. As a result, the uvp-monitor process fails to be run. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Domain0 fails to obtain in-band information about the VM. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -505,6 +418,205 @@
     <t xml:space="preserve">The "HWADDR=xx:xx:xx:xx" configuration option is missing in the VM NIC configuration file ifcfg-ethX. After the VM is restarted, the NIC fails to determine its name based on the MAC address in the ifcfg-ethX file. </t>
   </si>
   <si>
+    <t xml:space="preserve">Add the "HWADDR=xx:xx:xx:xx" configuration option to the /etc/sysconfig/network-scripts/ifcfg-ethX file. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contact OS vendors to obtain the corrective patch.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The actual free memory of the VM is smaller than the memory allocated by Xen hypervisor, and the VM sometimes crashes. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Log in to the VM, and run the lsmod | grep xen command to check whether the VM is armed with the Xen front-end driver. If "xen_vnif", "xen_vbd", and "xen_platform_pci" are displayed in the command output, the VM is armed with the Xen front-end driver. If the VM is not armed with the Xen front-end driver, do not use this VM any more. 
+2. Run the fdisk -l command to check whether the VM has two disk devices /dev/xvda and /dev/sda. Run the ifconfig –a command to check whether the VM has two NICs with identical MAC addresses. 
+3. If there are two disk devices on the VM, add "ide0=noprobe hdc=noprobe" to the /boot/grub/menu.lst file to disable the IDE disk. 
+4. If there are two NICs on the VM, add the following configurations at the end of the /etc/modprobe.d/blacklist.conf file to disable the 8139 NIC. 
+alias 8139cp off
+install 8139cp :
+alias 8139too off
+install 8139too :
+5. Run the mkinitrd -f /boot/initrd-$(uname -r).img $(uname -r) --with=xen_vbd --with=xen_vnif command to add the Xen front-end driver to the initrd file. 
+6. Restart the VM.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=72978b2fe2f2cdf9f319c6c6dcdbe92b38de2be2
+http://git.kernel.org/cgit/linux/kernel/git/tip/tip.git/commit/?id=c4288334818c81c946acb23d2319881f58c3d497</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add the following configurations at the end of the /etc/modprobe.d/blacklist.conf file to disable the 8139 NIC during the VM startup: 
+alias 8139cp off
+install 8139cp :
+alias 8139too off
+install 8139too :
+2. Restart the VM for the new configurations to take effect. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The live migration, snapshot, or hibernation of the VM fails. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, a VM uses the Qemu-emulated IDE disks instead of Xen paravirtual disks. During live migration, snapshot, or hibernation, the VM needs to be suspended. Once the VM is suspended, the Qemu on the VM is expected to stop, and the IO in the cache is expected to be updated to the Qemu-emulated IDE disks. However, the Qemu-emulated IDE disks are unable to handle the IO update. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM is defective. The VM is armed with two NICs whose MAC addresses are the same. One is the Qemu-emulated 8139 NIC; the other is the Xen paravirtual NIC. If these two NICs obtain IP addresses through DHCP, they may be assigned the same IP address. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The following operations issued by the Xenstore watch fail: 
+VM reboot 
+Live migration 
+Hibernation 
+Snapshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. If the Xen Hypervisor issues a hibernation operation to a VM, the Xenstore watch of the VM will be deregistered. However, the Xenstore watch is unable to handle VM hibernation failures. That is, if the hibernation of the VM fails, the Xenstore watch that is deregistered during the hibernation does not re-register with the kernel. As a result, the subsequent operations issued by the Xenstore watch fail. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.4, 6.5, 6.6, 6.7, 7.1, and 7.2 (32-bit and 64 bit) 
+CentOS 6.8 (64-bit) 
+Debian 6, 7, and 8
+Fedora 23 (64-bit)
+Oracle Linux 7.2 (64-bit)
+Red Hat Enterprise Linux 6.4 (32-bit and 64-bit)
+Red Hat Enterprise Linux 7.1 and 7.2 (64-bit)
+Versions 6.6, 6.7, and 7 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux
+Ubuntu 12, 13, 14, and 15
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The front-end NIC driver of a VM is defective: When you use the host to uninstall a down NIC from a VM, the front-end NIC driver of the VM calls the napi synchronization function. Executing this function causes the xenwatch thread to enter the D state. </t>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/?id=274b045509175db0405c784be85e8cce116e6f7d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install the corrective patch. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">During the status switching of the front- and back-end virtual disk drivers, the virtual disk driver processes the xenwatch status at a wrong time sequence. To be more specific, during the live migration, hibernation, or wake-up of the VM, the virtual disk driver mistakenly processes the XenbusStateConnected state for one more time, causing the VM unresponsive. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The hibernation, wake-up, or live migration of the VM fails. </t>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/next/linux-next.git/commit/drivers/block/xen-blkfront.c?id=efd1535270c1deb0487527bf0c3c827301a69c93</t>
+  </si>
+  <si>
+    <t>http://xenbits.xen.org/gitweb/?p=xen.git;a=commitdiff;h=9c89dc95201ffed5fead17b35754bf9440fdbdc0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CoreOS 1010.5.0 
+CoreOS 1068.2.0 
+All Linux OS distributions with kernel 4.5.0 or 4.6.0 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CoreOS 1010.5.0 
+CoreOS 1068.2.0 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">After the down NIC is hot-plugged out, all virtualization features of the VM are not available, such as: 
+NIC hot plug
+Disk hot plug 
+VM shutdown 
+VM restart 
+VM live migration
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Install the corrective patch. 
+Suggestion: Do not hot-plug a down NIC out. If this defect is triggered, forcibly restart the VM. 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Red Hat Enterprise Linux 6.4 (32-bit)
+Versions 6.4 and 6.5 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux (64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The live migration, snapshot, or hibernation of the VM that uses Linux kernel 2.6.32 fails occasionally. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.5 (64-bit)
+EulerOS 2.1.RC5 (64-bit)
+Oracle Linux Server 6.3 to 6.5 (32-bit and 64-bit)
+Oracle Linux 6.7 (32-bit) 
+Oracle Linux 7.2 (64-bit) 
+Red Hat Enterprise Linux 6.6, 7.1, and 7.2 (64-bit) 
+Ubuntu server 12.04.5 (32-bit and 64-bit) 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.7 (64-bit)
+openSUSE 13.2 (64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>If a VM attempts to start up while the host CPU usage is high, the AP CPU may be scheduled to execute other tasks when its state is changing from online to active. In this case, if the boot CPU tries to migrate the kernel threads (for example, migration, ksoftirq, and watchdog threads) related to the hotplug thread of the AP CPU, the migration fails and these threads encounter a bug-on error.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.3, 6.8, and 7.0 (64-bit) 
+CentOS 6.4, 6.5, 6.6, and 6.7 (32-bit and 64-bit)
+Oracle Enterprise Linux 6.7 (32-bit) 
+Red Hat Enterprise Linux 6.4 and 6.6 (32-bit and 64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Xen front-end NIC driver is defective. Resource leak occurs when a VM deletes the granted references.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.3 and 6.8 (64-bit) 
+CentOS 6.4, 6.5, 6.6, and 6.7 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 6.4 and 6.6 (32-bit and 64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">A VM does not provide an interface (such as the /proc/xen/xenbus or /dev/xen/xenbus file) for user-space programs to access xenbus. As a result, the uvp-monitor process fails to be run. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain0 fails to obtain in-band information about the VM. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">During the VM restoration (after a VM is live migrated to the destination), the VM kernel restores the status of the Qemu-emulated device. This restoration operation lasts about 10s, during which, the VM fails to respond to network transmission requests. 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 12 (64-bit)
+Novell SuSE Linux Enterprise Server 12 SP1 (64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM does not respond when it is being restored using a snapshot. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The libxenstore component built in the VM is defective. The libxenstore.so library file of the VM accesses the /proc/xen/xenbus interface file by default. When the user-space program (for example, uvp-monitor process) registers the xenwatch through the libxenstore.so, the VM kernel reads and writes the Xenstore, which triggers a conflict with the RCU lock mechanism of the kernel process file system. </t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve"> </t>
     </r>
@@ -520,66 +632,52 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Add the "HWADDR=xx:xx:xx:xx" configuration option to the /etc/sysconfig/network-scripts/ifcfg-ethX file. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Contact OS vendors to obtain the corrective patch.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The actual free memory of the VM is smaller than the memory allocated by Xen hypervisor, and the VM sometimes crashes. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Log in to the VM, and run the lsmod | grep xen command to check whether the VM is armed with the Xen front-end driver. If "xen_vnif", "xen_vbd", and "xen_platform_pci" are displayed in the command output, the VM is armed with the Xen front-end driver. If the VM is not armed with the Xen front-end driver, do not use this VM any more. 
-2. Run the fdisk -l command to check whether the VM has two disk devices /dev/xvda and /dev/sda. Run the ifconfig –a command to check whether the VM has two NICs with identical MAC addresses. 
-3. If there are two disk devices on the VM, add "ide0=noprobe hdc=noprobe" to the /boot/grub/menu.lst file to disable the IDE disk. 
-4. If there are two NICs on the VM, add the following configurations at the end of the /etc/modprobe.d/blacklist.conf file to disable the 8139 NIC. 
-alias 8139cp off
-install 8139cp :
-alias 8139too off
-install 8139too :
-5. Run the mkinitrd -f /boot/initrd-$(uname -r).img $(uname -r) --with=xen_vbd --with=xen_vnif command to add the Xen front-end driver to the initrd file. 
-6. Restart the VM.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=72978b2fe2f2cdf9f319c6c6dcdbe92b38de2be2
-http://git.kernel.org/cgit/linux/kernel/git/tip/tip.git/commit/?id=c4288334818c81c946acb23d2319881f58c3d497</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Add the following configurations at the end of the /etc/modprobe.d/blacklist.conf file to disable the 8139 NIC during the VM startup: 
-alias 8139cp off
-install 8139cp :
-alias 8139too off
-install 8139too :
-2. Restart the VM for the new configurations to take effect. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The VM kernel is defective. If the Xen Hypervisor issues a hibernation operation to a VM, the XenStore watch of the VM will be deregistered. However, the XenStore watch is unable to handle VM hibernation failures. That is, if the hibernation of the VM fails, the XenStore watch that is deregistered during the hibernation does not re-register with the kernel. As a result, the subsequent operations issued by the XenStore watch fail. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The following operations issued by the XenStore watch fail: 
-VM reboot 
-Live migration 
-Hibernation 
-Snapshot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The live migration, snapshot, or hibernation of the VM fails. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">By default, a VM uses the Qemu-emulated IDE disks instead of Xen paravirtual disks. During live migration, snapshot, or hibernation, the VM needs to be suspended. Once the VM is suspended, the Qemu on the VM is expected to stop, and the IO in the cache is expected to be updated to the Qemu-emulated IDE disks. However, the Qemu-emulated IDE disks are unable to handle the IO update. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The VM is defective. The VM is armed with two NICs whose MAC addresses are the same. One is the Qemu-emulated 8139 NIC; the other is the Xen paravirtual NIC. If these two NICs obtain IP addresses through DHCP, they may be assigned the same IP address. </t>
+    <t xml:space="preserve">CentOS 5.11, 6.4, 6.5, 6.6, 6.7, 7.1, and 7.2 (32-bit and 64 bit) 
+CentOS 6.3, 6.8, and 7.0 (64-bit)
+Debian GNU and Linux 7.1.0 (32-bit and 64-bit)
+EulerOS 2.1.RC5 (64-bit)
+Fedora 23 (64-bit)
+Novell SuSE Linux Enterprise Server 11 SP3 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 11 SP4 (64-bit)
+Oracle Linux 6.4 and 6.7 (32-bite and 64-bit) 
+Oracle Linux 7.0 and 7.2 (64-bit)
+Red Hat Enterprise Linux 6.4 and 6.6 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 7.0, 7.1, and 7.2 (64-bit) 
+Ubuntu 12
+Ubuntu server 14.04.3 (32-bit) 
+Ubuntu server 14.04.4 (32-bit and 64-bit) 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Debian GNU and Linux 8.2.0 (32-bit) 
+Fedora 23 (64-bit) 
+Oracle Linux 7.2 (64-bit) 
+Ubuntu server 14.04.3 (32-bit) 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OS with Linux kernel 4.6 or a later version, for example, 64-bit CoreOS Stable 1068.2.0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The kernel of the VM OS enables the "Invalidate Processor-Context Identifier" feature of the Intel Haswell, causing a compatibility failure. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM crashes during the startup. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">No official corrective patch is available. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Perform the following steps to disable the "Invalidate Processor-Context Identifier" feature: 
+1. Start the VM and log in to the VNC of the VM. On the displayed GRUB menu page, press any key except Enter to stay at the GRUB menu page. 
+2. Select a to-be-started item and press E to edit this item. Then, add kernel parameter "noinvpcid" to this item. For example, if GRUB version 2 is used, suffix "noinvpcid" to the line starting with "linux", that is, "linux$suf /coreos/vmlinuz-a mount.usr=PARTUUID=$usr_uuid $linux_cmdline noinvpcid", and then save and restart the VM. 
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -587,7 +685,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -621,12 +719,6 @@
       <sz val="10.5"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -841,134 +933,113 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1419,10 +1490,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" customHeight="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="38"/>
+      <c r="C2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="46.5">
       <c r="A3" s="7" t="s">
@@ -1432,17 +1503,17 @@
     </row>
     <row r="4" spans="1:3" ht="114" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="38"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:3" ht="46.5">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="8"/>
@@ -1451,55 +1522,55 @@
       <c r="A7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3" ht="21" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="29"/>
     </row>
     <row r="11" spans="1:3" ht="34.5" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:3" ht="31.5" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="30"/>
     </row>
     <row r="13" spans="1:3" ht="13.5" customHeight="1">
       <c r="A13" s="9"/>
@@ -1519,10 +1590,10 @@
     </row>
     <row r="16" spans="1:3" ht="34.5" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="28"/>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="11" t="s">
@@ -1581,60 +1652,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.375" customWidth="1"/>
-    <col min="2" max="2" width="48" style="1" customWidth="1"/>
+    <col min="2" max="2" width="41.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="47.5" customWidth="1"/>
     <col min="4" max="4" width="31.375" customWidth="1"/>
     <col min="5" max="5" width="61.5" style="17" customWidth="1"/>
-    <col min="6" max="6" width="57.875" customWidth="1"/>
+    <col min="6" max="6" width="72.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="47.25">
+    <row r="2" spans="1:6" ht="63">
       <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>90</v>
+        <v>127</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>82</v>
       </c>
+      <c r="E2" s="22" t="s">
+        <v>81</v>
+      </c>
       <c r="F2" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="94.5">
@@ -1642,19 +1711,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>79</v>
+        <v>128</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="78.75">
@@ -1662,15 +1731,15 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="18" t="s">
@@ -1682,19 +1751,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>121</v>
+        <v>71</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>105</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="47.25">
@@ -1702,79 +1771,79 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="21" t="s">
         <v>67</v>
       </c>
+      <c r="E6" s="23" t="s">
+        <v>66</v>
+      </c>
       <c r="F6" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="94.5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="204.75">
       <c r="A7" s="18">
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>91</v>
+        <v>115</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="19" t="s">
         <v>63</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="157.5">
+    <row r="8" spans="1:6" ht="299.25">
       <c r="A8" s="18">
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>61</v>
+        <v>106</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="173.25">
+    <row r="9" spans="1:6" ht="157.5">
       <c r="A9" s="18">
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="21" t="s">
         <v>57</v>
       </c>
+      <c r="E9" s="23" t="s">
+        <v>56</v>
+      </c>
       <c r="F9" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="94.5">
@@ -1782,27 +1851,27 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="21" t="s">
         <v>52</v>
       </c>
+      <c r="E10" s="23" t="s">
+        <v>51</v>
+      </c>
       <c r="F10" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="94.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="126">
       <c r="A11" s="18">
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>50</v>
+        <v>129</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>49</v>
@@ -1810,7 +1879,7 @@
       <c r="D11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F11" s="18" t="s">
@@ -1830,7 +1899,7 @@
       <c r="D12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="22" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="18" t="s">
@@ -1841,8 +1910,8 @@
       <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>93</v>
+      <c r="B13" s="24" t="s">
+        <v>130</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>41</v>
@@ -1850,7 +1919,7 @@
       <c r="D13" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="22" t="s">
         <v>39</v>
       </c>
       <c r="F13" s="18" t="s">
@@ -1861,7 +1930,7 @@
       <c r="A14" s="18">
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="24" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="18" t="s">
@@ -1870,7 +1939,7 @@
       <c r="D14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="23" t="s">
         <v>35</v>
       </c>
       <c r="F14" s="18" t="s">
@@ -1881,56 +1950,56 @@
       <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="24" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="22" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="78.75">
+    <row r="16" spans="1:6" ht="94.5">
       <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>94</v>
+      <c r="B16" s="24" t="s">
+        <v>132</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="22" t="s">
         <v>29</v>
       </c>
       <c r="F16" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="78.75">
+    <row r="17" spans="1:6" ht="94.5">
       <c r="A17" s="18">
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="18" t="s">
@@ -1942,183 +2011,260 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="E18" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="126">
+      <c r="A19" s="18">
+        <v>18</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="110.25">
+      <c r="A20" s="18">
+        <v>19</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="31.5">
+      <c r="A21" s="18">
+        <v>20</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="63">
+      <c r="A22" s="18">
+        <v>21</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="63">
+      <c r="A23" s="18">
+        <v>22</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="126">
-      <c r="A19" s="26">
-        <v>18</v>
-      </c>
-      <c r="B19" s="18" t="s">
+      <c r="E23" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="283.5">
+      <c r="A24" s="18">
+        <v>23</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="26" t="s">
+      <c r="D24" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F24" s="18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="126">
+      <c r="A25" s="18">
+        <v>24</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="126">
-      <c r="A20" s="28">
-        <v>19</v>
-      </c>
-      <c r="B20" s="26" t="s">
+    <row r="26" spans="1:6" ht="78.75">
+      <c r="A26" s="18">
+        <v>25</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="141.75">
+      <c r="A27" s="18">
+        <v>26</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="31.5">
-      <c r="A21" s="30">
-        <v>20</v>
-      </c>
-      <c r="B21" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="63">
-      <c r="A22" s="30">
-        <v>21</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="26" t="s">
+      <c r="F27" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="110.25">
+      <c r="A28" s="18">
+        <v>27</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D22" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="63">
-      <c r="A23" s="30">
-        <v>22</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="E23" s="32" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="110.25">
+      <c r="A29" s="18">
+        <v>28</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="26" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="315">
-      <c r="A24" s="30">
-        <v>23</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="29" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="126">
-      <c r="A25" s="30">
-        <v>24</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="D25" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="78.75">
-      <c r="A26" s="30">
-        <v>25</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="B28" s="34"/>
+      <c r="C29" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="126">
+      <c r="A30" s="18">
+        <v>29</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2133,8 +2279,10 @@
     <hyperlink ref="E17" r:id="rId8"/>
     <hyperlink ref="E7" r:id="rId9"/>
     <hyperlink ref="E22" r:id="rId10" display="https://bugzilla.redhat.com/show_bug.cgi?id=224662"/>
+    <hyperlink ref="E27" r:id="rId11"/>
+    <hyperlink ref="E28" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs/buglist: Upate the Bug list of Linux Distributions.
Signed-off-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -19,7 +19,8 @@
     <definedName name="_Hlt448738431" localSheetId="1">'Bug List'!$C$15</definedName>
     <definedName name="_Hlt448752930" localSheetId="1">'Bug List'!$F$12</definedName>
     <definedName name="_Hlt448771702" localSheetId="1">'Bug List'!$C$13</definedName>
-    <definedName name="_Hlt456345688" localSheetId="1">'Bug List'!$C$33</definedName>
+    <definedName name="_Hlt456345688" localSheetId="1">'Bug List'!$C$32</definedName>
+    <definedName name="_Hlt459023940" localSheetId="1">'Bug List'!$C$32</definedName>
     <definedName name="unitENG">[1]数据固化!$AB$4:$AB$21</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="174">
   <si>
     <t>Issue</t>
   </si>
@@ -56,44 +57,24 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">This is the first release. </t>
-  </si>
-  <si>
     <t>Changes between document issues are cumulative. The latest document issue contains all the changes made in earlier issues.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2016-04-19</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Overview</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The document describes the bugs of Linux distributions with the PVOPS kernel. </t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Intended Audience</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">This document is intended for Linux users who build the source code of UVP tools. 
-</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Document Structure</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>No.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">Bug sequence number. Bugs are listed according to the sequence of time when they were detected. </t>
@@ -365,9 +346,6 @@
     <t xml:space="preserve">The VM kernel is defective, causing uvp-monitor unable to be installed on the VM. </t>
   </si>
   <si>
-    <t xml:space="preserve">Domain0 fails to obtain the in-band information about the VM. </t>
-  </si>
-  <si>
     <t>Oracle Linux 6.7 (32-bit and 64-bit)</t>
   </si>
   <si>
@@ -398,7 +376,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FF010000"/>
+        <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -407,7 +385,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -623,7 +601,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color indexed="8"/>
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
@@ -658,26 +636,155 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OS with Linux kernel 4.6 or a later version, for example, 64-bit CoreOS Stable 1068.2.0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The kernel of the VM OS enables the "Invalidate Processor-Context Identifier" feature of the Intel Haswell, causing a compatibility failure. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The VM crashes during the startup. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">No official corrective patch is available. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Perform the following steps to disable the "Invalidate Processor-Context Identifier" feature: 
-1. Start the VM and log in to the VNC of the VM. On the displayed GRUB menu page, press any key except Enter to stay at the GRUB menu page. 
-2. Select a to-be-started item and press E to edit this item. Then, add kernel parameter "noinvpcid" to this item. For example, if GRUB version 2 is used, suffix "noinvpcid" to the line starting with "linux", that is, "linux$suf /coreos/vmlinuz-a mount.usr=PARTUUID=$usr_uuid $linux_cmdline noinvpcid", and then save and restart the VM. 
+    <t>All Linux OS distributions with the ixgbevf driver earlier than version 2.14.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The VM NIC stops receiving or sending packets, causing the network connectivity to be unavailable. 
+2. No response is provided after commands (such as, ip link and ifconfig) used to obtain network device information are run. 
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">This defect has been fixed in ixgbevf 2.14.2. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upgrade the ixgbevf driver of the VM to 2.16.1 or a higher version. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.6, 6.7, and 6.8 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 6.6, 6.7, and 6.8 (32-bit and 64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. An IPI scheduling patch is not incorporated in the OS. As a result, CPU load balancing of the VM OS becomes tardy. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">In the same running environment (with the same configurations), the performance of an affected VM is poorer than that of a normal VM. According to the performance test statistics measured by Geekbench, the multi-thread processing performance of an affected VM decreases by about 50%. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/arch/x86/xen/smp.c?id=184748cc50b2dceb8287f9fb657eda48ff8fcfe7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Install the corrective patch. 
+Alternatively, you can perform the following steps to fix this defect: 
+1. Log in to the VM after you obtain the permission to access the VM from the VM user. 
+2. In the CLI of the VM, run the following command to open the menu.lst file. 
+vim /boot/grub/menu.lst
+3. Add configuration item "nohz=off" at the end of the kernel configuration item. Then save the configurations. 
+4. Restart the VM for the configurations to take effect.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Domain0 fails to obtain in-band information about the VM. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The ixgbevf NIC driver of a VM is defective: There is a low possibility that the NIC driver is deadlocked after the MTU of the VM NIC is modified. If such a deadlock occurs, all functions used to obtain network device information become unavailable and the network connectivity of the VM is interrupted. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the second release. 
+Newly discovered bugs are added in this document. Newly found OSs that are affected by these bugs are also added in this document. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">This document is intended for users who want to understand the bugs and bug impacts of Linux distributions. 
+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM may fail to start up. </t>
+  </si>
+  <si>
+    <t>Novell SUSE Linux Enterprise Server 11 SP4 64-bit (kernel version 3.0.101 -63)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. There is a race condition between functions kset_find_obj_hinted() and kobject_put of the kernel. In such a race condition, there is a possibility that the kobject is released but some threads still access the released kobject. As a result, the kernel encounters a panic error and the VM becomes unavailable. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM may fail to start up. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/?id=a49b7e82cab0f9b41f483359be83f44fbb6b4979</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Install the corrective patch. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ubuntu server 14.04 LTS 32-bit and 64-bit (kernel version 3.13.0-24-generic)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The VM kernel is defective. During the VM live migration, hibernation, wake-up on the Xen platform, the front-end NIC driver (xen-netfront) reconnects to or disconnects from the back-end NIC driver. During the disconnection and reconnection operations, the entries of the grant table leak. As a result, no entry of the grant table is available, triggering a bug-on error of the kernel.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a high possibility that the VM crashes during the live migration, hibernation, and wake-up of the VM. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=a5b5dc3ce4df4f05f4d81c7d3c56a7604b242093
+https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=2688fcb79498246d45a0fa5900e415bc97661b6f 
+https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=b7dd0e350e0bd4c0fddcc9b8958342700b00b168
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Novell SUSE Linux Enterprise Server 11 SP1 32-bit and 64-bit (kernel version 2.6.32.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. During the VM startup, the kernel module microcode needs to be loaded, but a pointer is repeatedly released in the kernel code. In this case, the mc pointer of the generic_load_microcode function points to a null address when the microcode module is loaded, thereby causing the VM to crash. </t>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/?h=linux-4.6.y&amp;id=5cdd2de0a76d0ac47f107c8a7b32d75d25768dc1</t>
+  </si>
+  <si>
+    <t>CentOS 6.3 32-bit and 64-bit (kernel version 2.6.32 -279)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. When a NIC is hot-plugged in, the front-end NIC driver (netfront) of the kernel calls functions at a wrong time sequence, causing the NIC status to become "IF_OPER_UNKNOWN". In this case, the system mistakenly determines that the NIC is operable. A time sequence error also occurs when a NIC is hot-plugged out. Due to this error, the system mistakenly considers the link of a deregistered NIC (netdev) as available, and accesses the deregistered NIC. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM may encounter a panic error when the NIC is hot-plugged in or out. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=8f4cccbbd92f2ad0ddbbc498ef7cee2a1c3defe9
+https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=6bc96d047fe32d76ef79f3195c52a542edf7c705
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016-04-19</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the first release. </t>
+  </si>
+  <si>
+    <t>02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The document describes the bugs of Linux distributions. </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016-08-16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -685,34 +792,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="29">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -736,16 +831,107 @@
       <sz val="12"/>
       <color indexed="12"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="48"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -756,89 +942,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color indexed="48"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -852,11 +962,11 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -885,12 +995,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.24994659260841701"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF006699"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -898,6 +1002,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.24994659260841701"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,14 +1040,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -949,116 +1059,108 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8"/>
-    <cellStyle name="超链接 2" xfId="2"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8"/>
+    <cellStyle name="超链接 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1472,10 +1574,10 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="21.25" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.625" style="4" customWidth="1"/>
@@ -1485,32 +1587,32 @@
   <sheetData>
     <row r="1" spans="1:3" ht="23.25">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="72" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="31" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="C2" s="31"/>
     </row>
     <row r="3" spans="1:3" ht="46.5">
       <c r="A3" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="114" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="31" t="s">
-        <v>16</v>
+        <v>150</v>
       </c>
       <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:3" ht="46.5">
       <c r="A5" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
@@ -1520,10 +1622,10 @@
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1">
       <c r="A7" s="14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C7" s="29"/>
     </row>
@@ -1532,16 +1634,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1">
       <c r="A9" s="14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" s="29"/>
     </row>
@@ -1550,7 +1652,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10" s="29"/>
     </row>
@@ -1559,16 +1661,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C11" s="29"/>
     </row>
     <row r="12" spans="1:3" ht="31.5" customHeight="1">
       <c r="A12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="30" t="s">
         <v>21</v>
-      </c>
-      <c r="B12" s="30" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="30"/>
     </row>
@@ -1591,7 +1693,7 @@
     <row r="16" spans="1:3" ht="34.5" customHeight="1">
       <c r="A16" s="5"/>
       <c r="B16" s="28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="28"/>
     </row>
@@ -1608,16 +1710,26 @@
     </row>
     <row r="18" spans="1:3" ht="48" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>11</v>
+        <v>171</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>12</v>
+        <v>173</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="24" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="24" customHeight="1"/>
     <row r="21" spans="1:3" ht="24" customHeight="1"/>
     <row r="22" spans="1:3" ht="24" customHeight="1"/>
@@ -1652,9 +1764,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1668,7 +1782,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75">
       <c r="A1" s="19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>2</v>
@@ -1691,19 +1805,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="94.5">
@@ -1711,19 +1825,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="78.75">
@@ -1731,19 +1845,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="94.5">
@@ -1751,19 +1865,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="47.25">
@@ -1771,19 +1885,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="204.75">
@@ -1791,19 +1905,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="299.25">
@@ -1811,19 +1925,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="157.5">
@@ -1831,19 +1945,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="94.5">
@@ -1851,19 +1965,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="126">
@@ -1871,19 +1985,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31.5">
@@ -1891,19 +2005,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="94.5">
@@ -1911,19 +2025,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="110.25">
@@ -1931,19 +2045,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="110.25">
@@ -1951,19 +2065,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="94.5">
@@ -1971,19 +2085,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="94.5">
@@ -1991,19 +2105,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="94.5">
@@ -2011,19 +2125,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="126">
@@ -2031,239 +2145,339 @@
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="110.25">
+      <c r="A20" s="24">
+        <v>19</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="31.5">
+      <c r="A21" s="25">
+        <v>20</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="63">
+      <c r="A22" s="25">
+        <v>21</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="63">
+      <c r="A23" s="25">
+        <v>22</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="283.5">
+      <c r="A24" s="25">
+        <v>23</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="126">
+      <c r="A25" s="25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="78.75">
+      <c r="A26" s="25">
+        <v>25</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="141.75">
+      <c r="A27" s="25">
+        <v>26</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="110.25">
+      <c r="A28" s="25">
+        <v>27</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="110.25">
+      <c r="A29" s="25">
+        <v>28</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="126">
+      <c r="A30" s="25">
+        <v>29</v>
+      </c>
+      <c r="B30" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="110.25">
-      <c r="A20" s="18">
-        <v>19</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="31.5">
-      <c r="A21" s="18">
-        <v>20</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="63">
-      <c r="A22" s="18">
-        <v>21</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="25" t="s">
+      <c r="C30" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F30" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="E22" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="63">
-      <c r="A23" s="18">
-        <v>22</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="283.5">
-      <c r="A24" s="18">
-        <v>23</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="126">
-      <c r="A25" s="18">
-        <v>24</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="78.75">
-      <c r="A26" s="18">
-        <v>25</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="141.75">
-      <c r="A27" s="18">
-        <v>26</v>
-      </c>
-      <c r="B27" s="18" t="s">
+    </row>
+    <row r="31" spans="1:6" ht="141.75">
+      <c r="A31" s="25">
+        <v>30</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="110.25">
-      <c r="A28" s="18">
-        <v>27</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="110.25">
-      <c r="A29" s="18">
-        <v>28</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="126">
-      <c r="A30" s="18">
-        <v>29</v>
-      </c>
-      <c r="B30" s="18" t="s">
+      <c r="D31" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="E31" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="F31" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="E30" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>148</v>
+    </row>
+    <row r="32" spans="1:6" ht="103.5" customHeight="1">
+      <c r="A32" s="25">
+        <v>31</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="117.75" customHeight="1">
+      <c r="A33" s="25">
+        <v>32</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="105" customHeight="1">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="141.75">
+      <c r="A35" s="25">
+        <v>34</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E35" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2281,8 +2495,9 @@
     <hyperlink ref="E22" r:id="rId10" display="https://bugzilla.redhat.com/show_bug.cgi?id=224662"/>
     <hyperlink ref="E27" r:id="rId11"/>
     <hyperlink ref="E28" r:id="rId12"/>
+    <hyperlink ref="E31" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs/buglist: Updates the Bug list of linux distributions.
Add the bugs of tty driver in kernel and qspinlocks of xen's vcpu in vm.
updates the bugs of netfront with napi schedule.

Signed-off-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="185">
   <si>
     <t>Issue</t>
   </si>
@@ -722,10 +722,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Ubuntu server 14.04 LTS 32-bit and 64-bit (kernel version 3.13.0-24-generic)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>The VM kernel is defective. During the VM live migration, hibernation, wake-up on the Xen platform, the front-end NIC driver (xen-netfront) reconnects to or disconnects from the back-end NIC driver. During the disconnection and reconnection operations, the entries of the grant table leak. As a result, no entry of the grant table is available, triggering a bug-on error of the kernel.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -766,11 +762,11 @@
   </si>
   <si>
     <t>01</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t>2016-04-19</t>
-    <phoneticPr fontId="16" type="noConversion"/>
+    <phoneticPr fontId="17" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">This is the first release. </t>
@@ -785,6 +781,63 @@
   </si>
   <si>
     <t>2016-08-16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016-09-30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is the third release. 
+Newly discovered bugs are added in this document. 
+The following newly found OSs that are affected by the bugs are added in this document (for details, see line 32). 
+CentOS 6.5 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.5 (32-bit and 64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CentOS 6.5 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.5 (32-bit and 64-bit)
+Ubuntu server 14.04 LTS 32-bit and 64-bit (kernel version 3.13.0-24-generic)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=7098296a362a96051fa120abf48f0095818b99cd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=707e59ba494372a90d245f18b0c78982caa88e48</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 12 SP1 (32-bit and 64-bit) 
+openSUSE 13.2 and 42.1 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 7.0 (32-bit and 64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The VM kernel is defective. The serial port driver of the VM kernel checks whether the cache in the TTY structure is null only when the flush_to_ldisc function is called for the first time. If the cache is not null, it is directly assigned for use. The cache is released and set to null after it is used. In the following procedure, the driver no longer checks the cache in the TTY structure. If multiple programs of the VM access the serial port at the same time, the driver does not check the cache in the TTY structure when the flush_to_ldisc function is recalled. In this case, the programs may access a null pointer, causing the VM to malfunction.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a low possibility that the VM encounters a black screen error or fails to respond. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ubuntu server 16.04 (64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The VM kernel has a defect. On a Xen virtualization platform, when the VM uses the qspinlocks, a CPU may try to kick another CPU that is spinning (because the spinning CPU has not initialized its kicker interrupt). However, due to this defect, a CPU may kick another CPU that has not completed the interrupt allocation during VM startup. As a result, the VM crashes, and the VNC encounters a black screen error.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM may fail to start up. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -792,7 +845,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="31">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -889,6 +942,12 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -982,6 +1041,18 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1040,10 +1111,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1052,20 +1123,20 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
@@ -1086,29 +1157,26 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1116,6 +1184,9 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1125,17 +1196,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1571,10 +1651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1592,10 +1672,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" customHeight="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" s="31"/>
+      <c r="B2" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" spans="1:3" ht="46.5">
       <c r="A3" s="7" t="s">
@@ -1605,17 +1685,17 @@
     </row>
     <row r="4" spans="1:3" ht="114" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="31"/>
+      <c r="C4" s="34"/>
     </row>
     <row r="5" spans="1:3" ht="46.5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="8"/>
@@ -1624,55 +1704,55 @@
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="29"/>
+      <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="29"/>
+      <c r="C8" s="32"/>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="29"/>
+      <c r="C9" s="32"/>
     </row>
     <row r="10" spans="1:3" ht="21" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="29"/>
+      <c r="C10" s="32"/>
     </row>
     <row r="11" spans="1:3" ht="34.5" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:3" ht="31.5" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="33"/>
     </row>
     <row r="13" spans="1:3" ht="13.5" customHeight="1">
       <c r="A13" s="9"/>
@@ -1692,10 +1772,10 @@
     </row>
     <row r="16" spans="1:3" ht="34.5" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="31"/>
     </row>
     <row r="17" spans="1:3" ht="24" customHeight="1">
       <c r="A17" s="11" t="s">
@@ -1708,29 +1788,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="48" customHeight="1">
+    <row r="18" spans="1:3" ht="93" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C18" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="54" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
-      <c r="A19" s="12" t="s">
+    <row r="20" spans="1:3" ht="24" customHeight="1">
+      <c r="A20" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="C20" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1"/>
+    </row>
     <row r="21" spans="1:3" ht="24" customHeight="1"/>
     <row r="22" spans="1:3" ht="24" customHeight="1"/>
     <row r="23" spans="1:3" ht="24" customHeight="1"/>
@@ -1739,6 +1829,7 @@
     <row r="26" spans="1:3" ht="24" customHeight="1"/>
     <row r="27" spans="1:3" ht="24" customHeight="1"/>
     <row r="28" spans="1:3" ht="24" customHeight="1"/>
+    <row r="29" spans="1:3" ht="24" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B16:C16"/>
@@ -1764,10 +1855,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2420,21 +2511,21 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="117.75" customHeight="1">
+    <row r="33" spans="1:6" ht="123" customHeight="1">
       <c r="A33" s="25">
         <v>32</v>
       </c>
       <c r="B33" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="D33" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="E33" s="25" t="s">
         <v>159</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>160</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>156</v>
@@ -2445,16 +2536,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="18" t="s">
         <v>161</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>162</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>151</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>156</v>
@@ -2465,19 +2556,59 @@
         <v>34</v>
       </c>
       <c r="B35" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="D35" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="E35" s="25" t="s">
         <v>166</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>167</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="191.25" customHeight="1">
+      <c r="A36" s="25">
+        <v>35</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="139.5" customHeight="1">
+      <c r="A37" s="25">
+        <v>36</v>
+      </c>
+      <c r="B37" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2496,8 +2627,10 @@
     <hyperlink ref="E27" r:id="rId11"/>
     <hyperlink ref="E28" r:id="rId12"/>
     <hyperlink ref="E31" r:id="rId13"/>
+    <hyperlink ref="E36" r:id="rId14"/>
+    <hyperlink ref="E37" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs/buglist: Update the os lists of flush_to_ldisc.
Signed-off-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -762,11 +762,11 @@
   </si>
   <si>
     <t>01</t>
-    <phoneticPr fontId="17" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t>2016-04-19</t>
-    <phoneticPr fontId="17" type="noConversion"/>
+    <phoneticPr fontId="16" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">This is the first release. </t>
@@ -814,30 +814,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>The VM kernel is defective. The serial port driver of the VM kernel checks whether the cache in the TTY structure is null only when the flush_to_ldisc function is called for the first time. If the cache is not null, it is directly assigned for use. The cache is released and set to null after it is used. In the following procedure, the driver no longer checks the cache in the TTY structure. If multiple programs of the VM access the serial port at the same time, the driver does not check the cache in the TTY structure when the flush_to_ldisc function is recalled. In this case, the programs may access a null pointer, causing the VM to malfunction.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a low possibility that the VM encounters a black screen error or fails to respond. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ubuntu server 16.04 (64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The VM kernel has a defect. On a Xen virtualization platform, when the VM uses the qspinlocks, a CPU may try to kick another CPU that is spinning (because the spinning CPU has not initialized its kicker interrupt). However, due to this defect, a CPU may kick another CPU that has not completed the interrupt allocation during VM startup. As a result, the VM crashes, and the VNC encounters a black screen error.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM may fail to start up. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">Novell SuSE Linux Enterprise Server 12 SP1 (32-bit and 64-bit) 
 openSUSE 13.2 and 42.1 (32-bit and 64-bit) 
 Red Hat Enterprise Linux 7.0 (32-bit and 64-bit)
+Red Hat Enterprise Linux 7.2 (64-bit)
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The VM kernel is defective. The serial port driver of the VM kernel checks whether the cache in the TTY structure is null only when the flush_to_ldisc function is called for the first time. If the cache is not null, it is directly assigned for use. The cache is released and set to null after it is used. In the following procedure, the driver no longer checks the cache in the TTY structure. If multiple programs of the VM access the serial port at the same time, the driver does not check the cache in the TTY structure when the flush_to_ldisc function is recalled. In this case, the programs may access a null pointer, causing the VM to malfunction.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">There is a low possibility that the VM encounters a black screen error or fails to respond. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ubuntu server 16.04 (64-bit)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The VM kernel has a defect. On a Xen virtualization platform, when the VM uses the qspinlocks, a CPU may try to kick another CPU that is spinning (because the spinning CPU has not initialized its kicker interrupt). However, due to this defect, a CPU may kick another CPU that has not completed the interrupt allocation during VM startup. As a result, the VM crashes, and the VNC encounters a black screen error.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The VM may fail to start up. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -845,7 +846,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="34">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -938,12 +939,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1111,10 +1106,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1130,13 +1125,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
@@ -1157,26 +1152,29 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1184,37 +1182,34 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1653,9 +1648,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -1858,7 +1851,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2576,13 +2569,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="D36" s="18" t="s">
         <v>180</v>
-      </c>
-      <c r="D36" s="18" t="s">
-        <v>181</v>
       </c>
       <c r="E36" s="25" t="s">
         <v>177</v>
@@ -2596,13 +2589,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>182</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="D37" s="18" t="s">
         <v>183</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>184</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>178</v>

</xml_diff>

<commit_message>
docs/buglist: Update the os lists of flush_to_ldisc bug.
Signed-off-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -834,7 +834,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 12 SP1 (32-bit and 64-bit) 
+    <t xml:space="preserve">CentOS 7.2 (64-bit)
+Novell SuSE Linux Enterprise Server 12 SP1 (32-bit and 64-bit) 
 openSUSE 13.2 and 42.1 (32-bit and 64-bit) 
 Red Hat Enterprise Linux 7.0 (32-bit and 64-bit)
 Red Hat Enterprise Linux 7.2 (64-bit)
@@ -1850,7 +1851,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
docs/buglist: Update the os lists for qspinlocks/user_space_xenbus/plug_in_vm_lvm.
Add three titles, as bellow:
1. xen/qspinlock: Don't kick CPU if IRQ is not initialized.
2. xenbus: don't look up transaction IDs for ordinary writes.
3. plug a disk of vm when it had been used in lvm.

Signed-off-by: uvptools@huawei.com
Reviewed-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="197">
   <si>
     <t>Issue</t>
   </si>
@@ -136,16 +136,6 @@
     <t xml:space="preserve">
 None.</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. When a program accesses a file system or network through an emulated device, the program performance deteriorates. 
-2. When a device has two accessible objects, the VM data consistency may be affected. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When a VM starts with default settings, the VM kernel detects and activates the Qemu-emulated device and the Xen back-end device at the same time. For example, xvda disk is configured for the VM, but both xvda and sda disks coexist on the VM and point to the same device. </t>
-  </si>
-  <si>
-    <t>Novell SuSE Linux Enterprise Server 11 SP3</t>
   </si>
   <si>
     <t>Xenstore patch: 
@@ -355,42 +345,13 @@
     <t xml:space="preserve">In the case of constant live migration, the VM may fail to respond after it is live migrated to the destination. </t>
   </si>
   <si>
-    <t>CentOS 5.11 (32-bit and 64-bit)</t>
-  </si>
-  <si>
     <t>CentOS 6.3 (64-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">The virtual disk of a VM is unable to handle VM suspension failures. If the VM fails to be suspended, the granted references of the virtual disk are not released. In this case, resuming the virtual disk causes a failure in applying for granted references. </t>
   </si>
   <si>
-    <t xml:space="preserve">https://bugzilla.redhat.com/show_bug.cgi?id=224662 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Install the corrective patch to reduce the possibility of this problem. </t>
-  </si>
-  <si>
-    <r>
-      <t>CentOS 5.11 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">32-bit and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>64-bit)</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">The "HWADDR=xx:xx:xx:xx" configuration option is missing in the VM NIC configuration file ifcfg-ethX. After the VM is restarted, the NIC fails to determine its name based on the MAC address in the ifcfg-ethX file. </t>
@@ -457,22 +418,6 @@
     <t xml:space="preserve">The VM kernel is defective. If the Xen Hypervisor issues a hibernation operation to a VM, the Xenstore watch of the VM will be deregistered. However, the Xenstore watch is unable to handle VM hibernation failures. That is, if the hibernation of the VM fails, the Xenstore watch that is deregistered during the hibernation does not re-register with the kernel. As a result, the subsequent operations issued by the Xenstore watch fail. </t>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 6.4, 6.5, 6.6, 6.7, 7.1, and 7.2 (32-bit and 64 bit) 
-CentOS 6.8 (64-bit) 
-Debian 6, 7, and 8
-Fedora 23 (64-bit)
-Oracle Linux 7.2 (64-bit)
-Red Hat Enterprise Linux 6.4 (32-bit and 64-bit)
-Red Hat Enterprise Linux 7.1 and 7.2 (64-bit)
-Versions 6.6, 6.7, and 7 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux
-Ubuntu 12, 13, 14, and 15
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">The front-end NIC driver of a VM is defective: When you use the host to uninstall a down NIC from a VM, the front-end NIC driver of the VM calls the napi synchronization function. Executing this function causes the xenwatch thread to enter the D state. </t>
-  </si>
-  <si>
     <t>https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/?id=274b045509175db0405c784be85e8cce116e6f7d</t>
   </si>
   <si>
@@ -494,22 +439,6 @@
     <t xml:space="preserve">CoreOS 1010.5.0 
 CoreOS 1068.2.0 
 All Linux OS distributions with kernel 4.5.0 or 4.6.0 
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CoreOS 1010.5.0 
-CoreOS 1068.2.0 
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">After the down NIC is hot-plugged out, all virtualization features of the VM are not available, such as: 
-NIC hot plug
-Disk hot plug 
-VM shutdown 
-VM restart 
-VM live migration
 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -550,22 +479,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 6.3, 6.8, and 7.0 (64-bit) 
-CentOS 6.4, 6.5, 6.6, and 6.7 (32-bit and 64-bit)
-Oracle Enterprise Linux 6.7 (32-bit) 
-Red Hat Enterprise Linux 6.4 and 6.6 (32-bit and 64-bit)
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>The Xen front-end NIC driver is defective. Resource leak occurs when a VM deletes the granted references.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CentOS 6.3 and 6.8 (64-bit) 
-CentOS 6.4, 6.5, 6.6, and 6.7 (32-bit and 64-bit) 
-Red Hat Enterprise Linux 6.4 and 6.6 (32-bit and 64-bit)
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -610,32 +524,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 5.11, 6.4, 6.5, 6.6, 6.7, 7.1, and 7.2 (32-bit and 64 bit) 
-CentOS 6.3, 6.8, and 7.0 (64-bit)
-Debian GNU and Linux 7.1.0 (32-bit and 64-bit)
-EulerOS 2.1.RC5 (64-bit)
-Fedora 23 (64-bit)
-Novell SuSE Linux Enterprise Server 11 SP3 (32-bit and 64-bit)
-Novell SuSE Linux Enterprise Server 11 SP4 (64-bit)
-Oracle Linux 6.4 and 6.7 (32-bite and 64-bit) 
-Oracle Linux 7.0 and 7.2 (64-bit)
-Red Hat Enterprise Linux 6.4 and 6.6 (32-bit and 64-bit) 
-Red Hat Enterprise Linux 7.0, 7.1, and 7.2 (64-bit) 
-Ubuntu 12
-Ubuntu server 14.04.3 (32-bit) 
-Ubuntu server 14.04.4 (32-bit and 64-bit) 
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Debian GNU and Linux 8.2.0 (32-bit) 
-Fedora 23 (64-bit) 
-Oracle Linux 7.2 (64-bit) 
-Ubuntu server 14.04.3 (32-bit) 
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>All Linux OS distributions with the ixgbevf driver earlier than version 2.14.2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -681,10 +569,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">Domain0 fails to obtain in-band information about the VM. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">The ixgbevf NIC driver of a VM is defective: There is a low possibility that the NIC driver is deadlocked after the MTU of the VM NIC is modified. If such a deadlock occurs, all functions used to obtain network device information become unavailable and the network connectivity of the VM is interrupted. </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -792,14 +676,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>This is the third release. 
-Newly discovered bugs are added in this document. 
-The following newly found OSs that are affected by the bugs are added in this document (for details, see line 32). 
-CentOS 6.5 (32-bit and 64-bit)
-Red Hat Enterprise Linux 6.5 (32-bit and 64-bit)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CentOS 6.5 (32-bit and 64-bit)
 Red Hat Enterprise Linux 6.5 (32-bit and 64-bit)
 Ubuntu server 14.04 LTS 32-bit and 64-bit (kernel version 3.13.0-24-generic)</t>
@@ -826,20 +702,199 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">When a VM starts with default settings, the VM kernel detects and activates the Qemu-emulated device and the Xen back-end device at the same time. For example, the xvda disk is configured for the VM, but both xvda and sda disks coexist on the VM and point to the same device. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>The VM kernel has a defect. On a Xen virtualization platform, when the VM uses the qspinlocks, a CPU may try to kick another CPU that is spinning (because the spinning CPU has not initialized its kicker interrupt). However, due to this defect, a CPU may kick another CPU that has not completed the interrupt allocation during VM startup. As a result, the VM crashes, and the VNC encounters a black screen error.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">The VM may fail to start up. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">CentOS 7.2 (64-bit)
-Novell SuSE Linux Enterprise Server 12 SP1 (32-bit and 64-bit) 
+    <t>2016-11-07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is the fourth release. 
+Newly discovered bugs are added in this document: 
+Bug 37 — Hot-plugging disks in use through the host times out and fails. 
+Bug 38 — User-space programs of VMs running on Xen fail to access the Xenstore and the uvp-monitor process fails to run, due to the defect of the xenbus module. 
+Newly found OSs that are affected by existing bugs are added in this document. 
+For details, see the OSs affected by bugs 6, 7, 13, 15, 16, 19, 20, 23, 26, 28, and 35.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CentOS 5.11 (32-bit and 64-bit) 
+Novell SuSE Linux Enterprise Server 11 SP1 and SP2 
+Red Hat Enterprise Linux 5.11 (32-bit and 64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 5.11 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 5.11 (32-bit and 64-bit) </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CentOS 5.11 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 5.11 (32-bit and 64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CoreOS 1010.5.0
+CoreOS 1068.2.0
+CoreOS 1122.2.0
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All Linux OS distributions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The operation of hot-plugging disks in use times out and fails.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No official corrective patch is available.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">A defect is introduced to the xenbus module during the modification of the VM kernel. Due to this defect, user-space programs of VMs running on Xen fail to access the Xenstore, and the uvp-monitor process fails to run as well. 
+Link to the patch that introduces this defect: 
+https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/drivers/xen/xenbus/xenbus_dev_frontend.c?h=linux-4.7.y&amp;id=0beef634b86a1350c31da5fcc2992f0d7c8a622b
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User-space programs fail to access the Xenstore, and the uvp-monitor process fails to run.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Install the corrective patch.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/drivers/xen/xenbus/xenbus_dev_frontend.c?h=linux-4.7.y&amp;id=b035f15daf750e1594964d68889e0de5c3014922</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, 6.7, 7.0, 7.1, and 7.2 (32-bit and 64-bit) 
+CentOS 6.8 (64-bit)
+Debian 6, 7, and 8
+Fedora 23 (64-bit)
+Oracle Linux 6.6, 6.7, and 7.0 (32-bit and 64-bit) 
+Oracle Linux 7.2 (64-bit)
+Red Hat Enterprise Linux 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, 6.7, and 7.0 (32-bit and 64-bit)
+Red Hat Enterprise Linux 7.1 and 7.2 (64-bit)
+Versions 6.6, 6.7, and 7 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux
+Ubuntu 12, 13, 14, and 15
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 5.11, 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, 6.7, 7.1, and 7.2 (32-bit and 64-bit) 
+CentOS 6.8 and 7.0 (64-bit)
+Debian GNU and Linux 7.1.0 (32-bit and 64-bit)
+EulerOS 2.1.RC5 (64-bit)
+Fedora 23 (64-bit)
+Novell SuSE Linux Enterprise Server 11 SP3 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 11 SP4 (64-bit)
+Oracle Linux 6.4 and 6.7 (32-bite and 64-bit) 
+Oracle Linux 7.0 and 7.2 (64-bit)
+Red Hat Enterprise Linux 5.11, 6.1, 6.2, 6.3, 6.4, 6.5, and 6.6 (32-bit and 64-bit) 
+Red Hat Enterprise Linux 7.0, 7.1, and 7.2 (64-bit)
+Ubuntu 12
+Ubuntu server 14.04.3 (32-bit) 
+Ubuntu server 14.04.4 (32-bit and 64-bit) 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Novell SuSE Linux Enterprise Server 11 SP1, SP2, and SP3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. When a program accesses a file system or network through an emulated device, the program performance deteriorates. 
+2. When a device has two accessible objects, the VM data consistency may be affected, and querying disk information fails. 
+3. The live migration, memory snapshot, or hibernation of the VM fails.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, and 6.7 (32-bit and 64-bit) 
+CentOS 6.8 and 7.0 (64-bit)
+Oracle Enterprise Linux 6.7 (32-bit) 
+Red Hat Enterprise Linux 6.1, 6.2, 6.3, 6.4, 6.5, and 6.6 (32-bit and 64-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CentOS 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, and 6.7 (32-bit and 64-bit) 
+CentOS 6.8 (64-bit) 
+Red Hat Enterprise Linux 6.1, 6.2, 6.3, 6.4, 6.5 and 6.6 (32-bit and 64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Debian GNU and Linux 8.2.0 (32-bit and 64-bit) 
+Fedora 23 (64-bit) 
+Oracle Linux 7.2 (64-bit) 
+Ubuntu server 14.04.2 (32-bit and 64-bit) 
+Ubuntu server 14.04.3 (32-bit)
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. After the down NIC is hot-plugged out, all virtualization features of the VM are not available, such as: 
+NIC hot plug
+Disk hot plug 
+VM shutdown 
+VM restart 
+VM live migration
+2. The live migration, hibernation, wake-up, or snapshot of the VM with a down NIC fails.
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 12 SP1 (32-bit and 64-bit) 
 openSUSE 13.2 and 42.1 (32-bit and 64-bit) 
-Red Hat Enterprise Linux 7.0 (32-bit and 64-bit)
-Red Hat Enterprise Linux 7.2 (64-bit)
+CentOS 7.0 and 7.2 (32-bit and 64-bit)
+Red Hat Enterprise Linux 7.0 and 7.2 (32-bit and 64-bit) 
+Ubuntu server 16.04 (32-bit and 64-bit)
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">VMs have a restriction on device hot plug. Due to this restriction, when the host issues an operation of hot-plugging disks in use (for example, disks that have been mounted to a file system or added to a logical volume) to VMs, disk hot plug times out and fails. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The front-end NIC driver of a VM is defective: When you use the host to uninstall a down NIC from a VM or initiate hibernation, wake-up, live migration, or snapshot for a VM whose NIC is down, the front-end NIC driver of the VM calls the napi synchronization function. Executing this function causes the xenwatch thread to enter the D state. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Before hot-plugging a disk out of a VM, ensure that the disk is not in use. For example, if both xvde and xvdf disks are in logical volume VolGroup00, and you need to hot-plug the xvde disk, perform the following operations:  
+1. Run the lvremove /dev/VolGroup00/lvolhome command to delete the logical volume.  
+2. Use the host to issue the operation of hot-plugging the xvde disk to the VM. 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This is the third release. 
+Newly discovered bugs are added in this document. 
+The following newly found OSs that are affected by the bugs are added in this document (for details, see bug 32). 
+CentOS 6.5 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.5 (32-bit and 64-bit)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CoreOS 1122.2.0
+CoreOS 1122.3.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://bugzilla.redhat.com/show_bug.cgi?id=224662 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -847,7 +902,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="33">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1008,6 +1063,18 @@
       <family val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF010000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -1018,37 +1085,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF010000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
-      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1119,7 +1155,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1177,41 +1213,38 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1647,7 +1680,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1655,7 +1688,7 @@
   <cols>
     <col min="1" max="1" width="21.25" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="65.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="98.375" style="4" customWidth="1"/>
     <col min="4" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
@@ -1666,10 +1699,10 @@
     </row>
     <row r="2" spans="1:3" ht="72" customHeight="1">
       <c r="A2" s="5"/>
-      <c r="B2" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="34"/>
+      <c r="B2" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" ht="46.5">
       <c r="A3" s="7" t="s">
@@ -1679,17 +1712,17 @@
     </row>
     <row r="4" spans="1:3" ht="114" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" s="34"/>
+      <c r="B4" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="33"/>
     </row>
     <row r="5" spans="1:3" ht="46.5">
       <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="8"/>
@@ -1698,55 +1731,55 @@
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="31"/>
     </row>
     <row r="8" spans="1:3" ht="18.75" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="31"/>
     </row>
     <row r="9" spans="1:3" ht="18" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="31"/>
     </row>
     <row r="10" spans="1:3" ht="21" customHeight="1">
       <c r="A10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="31"/>
     </row>
     <row r="11" spans="1:3" ht="34.5" customHeight="1">
       <c r="A11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="32"/>
+      <c r="C11" s="31"/>
     </row>
     <row r="12" spans="1:3" ht="31.5" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="33"/>
+      <c r="C12" s="32"/>
     </row>
     <row r="13" spans="1:3" ht="13.5" customHeight="1">
       <c r="A13" s="9"/>
@@ -1766,12 +1799,12 @@
     </row>
     <row r="16" spans="1:3" ht="34.5" customHeight="1">
       <c r="A16" s="5"/>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="31"/>
-    </row>
-    <row r="17" spans="1:3" ht="24" customHeight="1">
+      <c r="C16" s="30"/>
+    </row>
+    <row r="17" spans="1:4" ht="24" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>0</v>
       </c>
@@ -1782,48 +1815,61 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="93" customHeight="1">
+    <row r="18" spans="1:4" ht="117" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="54" customHeight="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="93" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="54" customHeight="1">
       <c r="A20" s="12" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="24" customHeight="1"/>
-    <row r="22" spans="1:3" ht="24" customHeight="1"/>
-    <row r="23" spans="1:3" ht="24" customHeight="1"/>
-    <row r="24" spans="1:3" ht="24" customHeight="1"/>
-    <row r="25" spans="1:3" ht="24" customHeight="1"/>
-    <row r="26" spans="1:3" ht="24" customHeight="1"/>
-    <row r="27" spans="1:3" ht="24" customHeight="1"/>
-    <row r="28" spans="1:3" ht="24" customHeight="1"/>
-    <row r="29" spans="1:3" ht="24" customHeight="1"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="24" customHeight="1">
+      <c r="A21" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="24" customHeight="1">
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="1:4" ht="24" customHeight="1"/>
+    <row r="24" spans="1:4" ht="24" customHeight="1"/>
+    <row r="25" spans="1:4" ht="24" customHeight="1"/>
+    <row r="26" spans="1:4" ht="24" customHeight="1"/>
+    <row r="27" spans="1:4" ht="24" customHeight="1"/>
+    <row r="28" spans="1:4" ht="24" customHeight="1"/>
+    <row r="29" spans="1:4" ht="24" customHeight="1"/>
+    <row r="30" spans="1:4" ht="24" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B16:C16"/>
@@ -1849,11 +1895,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1865,23 +1909,23 @@
     <col min="6" max="6" width="72.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75">
-      <c r="A1" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:6" ht="30.75" customHeight="1">
+      <c r="A1" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="27" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1890,19 +1934,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="94.5">
@@ -1910,19 +1954,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="78.75">
@@ -1930,19 +1974,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>42</v>
+        <v>66</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="94.5">
@@ -1950,19 +1994,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="47.25">
@@ -1970,36 +2014,36 @@
         <v>5</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="204.75">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="236.25">
       <c r="A7" s="18">
         <v>6</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>54</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>22</v>
@@ -2010,16 +2054,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>136</v>
+        <v>183</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>55</v>
+        <v>94</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>52</v>
       </c>
       <c r="F8" s="18" t="s">
         <v>22</v>
@@ -2030,19 +2074,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>48</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="94.5">
@@ -2050,19 +2094,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="126">
@@ -2070,19 +2114,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="31.5">
@@ -2090,16 +2134,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>22</v>
@@ -2109,36 +2153,36 @@
       <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>124</v>
+      <c r="B13" s="21" t="s">
+        <v>114</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="110.25">
+    <row r="14" spans="1:6" ht="173.25">
       <c r="A14" s="18">
         <v>13</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>33</v>
+      <c r="B14" s="21" t="s">
+        <v>184</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>32</v>
+        <v>166</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="18" t="s">
@@ -2149,11 +2193,11 @@
       <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>27</v>
@@ -2165,15 +2209,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="94.5">
+    <row r="16" spans="1:6" ht="110.25">
       <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>126</v>
+      <c r="B16" s="21" t="s">
+        <v>186</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>25</v>
@@ -2185,18 +2229,18 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="94.5">
+    <row r="17" spans="1:6" ht="90.75" customHeight="1">
       <c r="A17" s="18">
         <v>16</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>128</v>
+        <v>187</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>23</v>
@@ -2210,19 +2254,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="126">
@@ -2230,379 +2274,419 @@
         <v>18</v>
       </c>
       <c r="B19" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="110.25">
+      <c r="A20" s="21">
+        <v>19</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="47.25" customHeight="1">
+      <c r="A21" s="22">
+        <v>20</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="63">
+      <c r="A22" s="22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="63">
+      <c r="A23" s="22">
+        <v>22</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="283.5">
+      <c r="A24" s="22">
+        <v>23</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="126">
+      <c r="A25" s="22">
+        <v>24</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="78.75">
+      <c r="A26" s="22">
+        <v>25</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="189">
+      <c r="A27" s="22">
+        <v>26</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="110.25">
+      <c r="A28" s="22">
+        <v>27</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="110.25">
+      <c r="A29" s="22">
+        <v>28</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="126">
+      <c r="A30" s="22">
+        <v>29</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="141.75">
+      <c r="A31" s="22">
+        <v>30</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="110.25">
-      <c r="A20" s="24">
-        <v>19</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="31.5">
-      <c r="A21" s="25">
-        <v>20</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" s="18" t="s">
+    </row>
+    <row r="32" spans="1:6" ht="103.5" customHeight="1">
+      <c r="A32" s="22">
+        <v>31</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="123" customHeight="1">
+      <c r="A33" s="22">
+        <v>32</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="105" customHeight="1">
+      <c r="A34" s="22">
+        <v>33</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="63">
-      <c r="A22" s="25">
-        <v>21</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="63">
-      <c r="A23" s="25">
-        <v>22</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="283.5">
-      <c r="A24" s="25">
-        <v>23</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" s="18" t="s">
+      <c r="F34" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="141.75">
+      <c r="A35" s="22">
+        <v>34</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="191.25" customHeight="1">
+      <c r="A36" s="22">
+        <v>35</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="126">
-      <c r="A25" s="25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="78.75">
-      <c r="A26" s="25">
-        <v>25</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="141.75">
-      <c r="A27" s="25">
-        <v>26</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E27" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="110.25">
-      <c r="A28" s="25">
-        <v>27</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="110.25">
-      <c r="A29" s="25">
-        <v>28</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="126">
-      <c r="A30" s="25">
-        <v>29</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D30" s="18" t="s">
+    </row>
+    <row r="37" spans="1:6" ht="139.5" customHeight="1">
+      <c r="A37" s="22">
+        <v>36</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="141.75">
-      <c r="A31" s="25">
-        <v>30</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="E31" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="103.5" customHeight="1">
-      <c r="A32" s="25">
-        <v>31</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E32" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="123" customHeight="1">
-      <c r="A33" s="25">
-        <v>32</v>
-      </c>
-      <c r="B33" s="18" t="s">
+      <c r="E37" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="94.5">
+      <c r="A38" s="22">
+        <v>37</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D33" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="105" customHeight="1">
-      <c r="A34" s="25">
-        <v>33</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="141.75">
-      <c r="A35" s="25">
-        <v>34</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>166</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="191.25" customHeight="1">
-      <c r="A36" s="25">
-        <v>35</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="C36" s="18" t="s">
+      <c r="E38" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="157.5">
+      <c r="A39" s="22">
+        <v>38</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" s="18" t="s">
         <v>179</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="E39" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F39" s="18" t="s">
         <v>180</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="F36" s="29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="139.5" customHeight="1">
-      <c r="A37" s="25">
-        <v>36</v>
-      </c>
-      <c r="B37" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="F37" s="29" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs/buglist: Modify the affected OS of missing 0.5GB of RAM
Fedora 23, EulerOS, ubuntu 12 and 14 had no affected.

Signed-off-by: uvptools@huawei.com
Reviewed-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -250,17 +250,13 @@
     <t xml:space="preserve">Install the corrective patch.</t>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 7.0 (64-bit)
+    <t xml:space="preserve">CentOS 7.1/7.2 (32-bit)
+CentOS 7.0, 7.1, and 7.2 (64-bit)
 Debian GNU and Linux 7.1.0 (32-bit and 64-bit)
-EulerOS 2.1.RC5 (64-bit)
-Fedora 23 (64-bit)
 Novell SuSE Linux Enterprise Server 12 SP1 (64-bit)
 Oracle Linux 6.4 and 6.7 (32-bit and 64-bit) 
 Oracle Linux 7.0 and 7.2 (64-bit)
-Red Hat Enterprise Linux 7.0, 7.1, and 7.2 (64-bit)
-Ubuntu 12
-Ubuntu server 14.04.3 (32-bit) 
-Ubuntu server 14.04.4 (32-bit and 64-bit) </t>
+Red Hat Enterprise Linux 7.0, 7.1, and 7.2 (64-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">When a VM calculates its maximum free memory, it counts the MMIO hole in. Therefore, the calculated free memory is greater than the actual free memory of the VM, triggering a balloon-out of the VM memory.</t>
@@ -771,12 +767,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="思源黑体 CN Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -792,21 +789,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <family val="0"/>
-      <charset val="134"/>
     </font>
     <font>
       <b val="true"/>
@@ -827,6 +809,7 @@
       <color rgb="FF0000FF"/>
       <name val="思源黑体 CN Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -834,6 +817,7 @@
       <color rgb="FF3366FF"/>
       <name val="思源黑体 CN Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -860,6 +844,7 @@
       <sz val="11"/>
       <name val="思源黑体 CN Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -970,7 +955,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -994,95 +979,84 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1090,15 +1064,23 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1106,40 +1088,22 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="常规 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="超链接 2" xfId="22" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1353,69 +1317,69 @@
       <c r="C14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1457,791 +1421,791 @@
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="47.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="47.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="21" width="70.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="83.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="70.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="83.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="n">
+      <c r="A2" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="n">
+      <c r="A3" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="n">
+      <c r="A4" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="n">
+      <c r="A5" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="23" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="n">
+      <c r="A6" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="23" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="236.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="n">
+      <c r="A7" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="23" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="141.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="n">
+    <row r="8" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="157.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="n">
+      <c r="A9" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="n">
+      <c r="A10" s="23" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="24" t="s">
+      <c r="F10" s="23" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="n">
+      <c r="A11" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="n">
+      <c r="A12" s="23" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="n">
+      <c r="A13" s="23" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="173.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="n">
+      <c r="A14" s="23" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="23" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="n">
+      <c r="A15" s="23" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="n">
+      <c r="A16" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="n">
+      <c r="A17" s="23" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="n">
+      <c r="A18" s="23" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="n">
+      <c r="A19" s="23" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="n">
+      <c r="A20" s="23" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="23" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="25" t="n">
+      <c r="A21" s="24" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="25" t="n">
+      <c r="A22" s="24" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="23" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="n">
+      <c r="A23" s="24" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="24" t="s">
+      <c r="D23" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="23" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="283.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="25" t="n">
+      <c r="A24" s="24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="24" t="s">
+      <c r="F24" s="23" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="25" t="n">
+      <c r="A25" s="24" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25" t="n">
+      <c r="A26" s="24" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="24" t="s">
+      <c r="F26" s="23" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="189" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25" t="n">
+      <c r="A27" s="24" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="23" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="25" t="n">
+      <c r="A28" s="24" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="24" t="s">
+      <c r="D28" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="F28" s="24" t="s">
+      <c r="F28" s="23" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25" t="n">
+      <c r="A29" s="24" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="23" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="25" t="n">
+      <c r="A30" s="24" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="F30" s="24" t="s">
+      <c r="F30" s="23" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25" t="n">
+      <c r="A31" s="24" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="24" t="s">
         <v>156</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="23" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="103.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="25" t="n">
+      <c r="A32" s="24" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="24" t="s">
         <v>161</v>
       </c>
-      <c r="F32" s="24" t="s">
+      <c r="F32" s="23" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="123" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25" t="n">
+      <c r="A33" s="24" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F33" s="23" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="25" t="n">
+      <c r="A34" s="24" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="F34" s="24" t="s">
+      <c r="F34" s="23" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25" t="n">
+      <c r="A35" s="24" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="D35" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="23" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="191.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="25" t="n">
+      <c r="A36" s="24" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="D36" s="24" t="s">
+      <c r="D36" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E36" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="F36" s="30" t="s">
+      <c r="F36" s="23" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="139.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25" t="n">
+      <c r="A37" s="24" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="27" t="s">
         <v>177</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="D37" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="F37" s="23" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="25" t="n">
+      <c r="A38" s="24" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="D38" s="24" t="s">
+      <c r="D38" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="F38" s="24" t="s">
+      <c r="F38" s="23" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="157.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="25" t="n">
+      <c r="A39" s="24" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="23" t="s">
         <v>185</v>
       </c>
-      <c r="D39" s="24" t="s">
+      <c r="D39" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="E39" s="25" t="s">
+      <c r="E39" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="F39" s="24" t="s">
+      <c r="F39" s="23" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
docs/buglist: Update the docs of Bug List.
Signed-off-by: uvptools@huawei.com
Reviewed-by: uvptools@huawei.com
</commit_message>
<xml_diff>
--- a/docs/Bug List of Linux Distributions.xlsx
+++ b/docs/Bug List of Linux Distributions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="About This Document" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="267">
   <si>
     <t xml:space="preserve">Overview</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-06-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the fifth release. </t>
   </si>
   <si>
     <t xml:space="preserve">04</t>
@@ -165,7 +174,9 @@
     <t xml:space="preserve">After the OS is installed, log in to the problem VM through the text-based user interface and install the corrective patch. </t>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 6, Oracle Linux 6, and Red Hat Enterprise Linux 6</t>
+    <t xml:space="preserve">Oracle Linux 5.7 (32-bit and 64-bit)
+Oracle Linux 5.8 (32-bit and 64-bit)
+CentOS 6, Oracle Linux 6, and Red Hat Enterprise Linux 6</t>
   </si>
   <si>
     <t xml:space="preserve">The USB subsystem of Linux kernel 2.6.32 may fail to be suspended, forcibly terminating the VM suspend procedure. </t>
@@ -213,6 +224,9 @@
     <t xml:space="preserve">Upgrade the kernel to version 2.6.32-358.23.2 or later. </t>
   </si>
   <si>
+    <t xml:space="preserve">CentOS 6, Oracle Linux 6, and Red Hat Enterprise Linux 6</t>
+  </si>
+  <si>
     <t xml:space="preserve">A VM supports only a maximum of 32 vCPUs due to the defective kernel. This bug has been fixed in the kernel of Red Hat 6.6.z. </t>
   </si>
   <si>
@@ -225,17 +239,30 @@
     <t xml:space="preserve">Install the corrective patch or upgrade the kernel to version 2.6.32-504.12.2 or later.</t>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, 6.7, 7.0, 7.1, and 7.2 (32-bit and 64-bit) 
+    <t xml:space="preserve">CentOS 6.1 (32-bit and 64-bit)
+CentOS 6.2 (32-bit and 64-bit)
+CentOS 6.3 (32-bit and 64-bit)
+CentOS 6.4 (32-bit and 64-bit)
+CentOS 6.5 (32-bit and 64-bit)
+CentOS 6.6 (32-bit and 64-bit)
+CentOS 6.7 (32-bit and 64-bit)
 CentOS 6.8 (64-bit)
-Debian 6, 7, and 8
-Fedora 23 (64-bit)
-Oracle Linux 6.6, 6.7, and 7.0 (32-bit and 64-bit) 
+CentOS 7.0, 7.1, 7.2, 7.3 (32-bit and 64-bit)
+Debian 6/7/8
+Fedora 22/23/24 (64-bit)
+Oracle Linux Server release 6.3 (32-bit and 64-bit)
 Oracle Linux 7.2 (64-bit)
-Red Hat Enterprise Linux 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, 6.7, and 7.0 (32-bit and 64-bit)
-Red Hat Enterprise Linux 7.1 and 7.2 (64-bit)
-Versions 6.6, 6.7, and 7 of the three operating systems: CentOS, Oracle Linux, and Red Hat Enterprise Linux
-Ubuntu 12, 13, 14, and 15
-</t>
+Red Hat Enterprise Linux 6.1 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.2 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.3 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.4 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.5 (32-bit and 64-bit)
+Red Hat Enterprise Linux 7.0 64-bit (kernel version: 3.10.0-514.6.1.el7.x86_64)
+Red Hat Enterprise Linux 7.0, 7.1, 7.2, 7.3 (32-bit and 64-bit)
+CentOS/Oracle Linux/Red Hat Enterprise Linux 6.6
+CentOS/Oracle Linux/Red Hat Enterprise Linux 6.7
+CentOS/Oracle Linux/Red Hat Enterprise Linux 7
+Ubuntu 12/13/14/15</t>
   </si>
   <si>
     <t xml:space="preserve">When a VM uses the snapshot restoration function, the kernel of the VM re-configures the memory address of vcpu_info, but does not inform the Xen hypervisor of the new memory address, thereby causing all other vCPUs (except vCPU0) unable to process interrupt signals. </t>
@@ -251,12 +278,14 @@
   </si>
   <si>
     <t xml:space="preserve">CentOS 7.1/7.2 (32-bit)
-CentOS 7.0, 7.1, and 7.2 (64-bit)
-Debian GNU and Linux 7.1.0 (32-bit and 64-bit)
+CentOS 7.0/7.1/7.2 (64-bit)
+Debian GNU/Linux 7.1.0 (32-bit and 64-bit)
 Novell SuSE Linux Enterprise Server 12 SP1 (64-bit)
-Oracle Linux 6.4 and 6.7 (32-bit and 64-bit) 
-Oracle Linux 7.0 and 7.2 (64-bit)
-Red Hat Enterprise Linux 7.0, 7.1, and 7.2 (64-bit)</t>
+Oracle Linux 6.4 (32-bit and 64-bit)
+Oracle Linux 6.7 (32-bit and 64-bit)
+Oracle Linux 7.0 (64-bit)
+Oracle Linux 7.2 (64-bit)
+Red Hat Enterprise Linux 7.0/7.1/7.2 (64-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">When a VM calculates its maximum free memory, it counts the MMIO hole in. Therefore, the calculated free memory is greater than the actual free memory of the VM, triggering a balloon-out of the VM memory.</t>
@@ -310,12 +339,13 @@
   <si>
     <t xml:space="preserve">CentOS 6.5 (64-bit)
 EulerOS 2.1.RC5 (64-bit)
-Oracle Linux Server 6.3 to 6.5 (32-bit and 64-bit)
-Oracle Linux 6.7 (32-bit) 
-Oracle Linux 7.2 (64-bit) 
-Red Hat Enterprise Linux 6.6, 7.1, and 7.2 (64-bit) 
-Ubuntu server 12.04.5 (32-bit and 64-bit) 
-</t>
+Oracle Linux Server release 6.3–6.5 (32-bit and 64-bit)
+Oracle Linux 6.7 (32-bit)
+Oracle Linux 7.2 (64-bit)
+Red Hat Enterprise Linux 6.6 (64-bit)
+Red Hat Enterprise Linux 7.1 (64-bit)
+Red Hat Enterprise Linux 7.2 (64-bit)
+Ubuntu Server 12.04.5 (32-bit and 64-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">The VM kernel is defective. During VM live migration, the VM kernel performs suspend and resume operations on Xen devices (front-end and back-end) and Qemu-emulated device. The operations on the Qemu-emulated device take about 10 seconds, during which the VM fails to respond to external requests. </t>
@@ -386,9 +416,10 @@
   <si>
     <t xml:space="preserve">CentOS 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, and 6.7 (32-bit and 64-bit) 
 CentOS 6.8 and 7.0 (64-bit)
+Oracle Enterprise Linux 5.8 (64-bit)
+Oracle Enterprise Linux 6.3 (64-bit)
 Oracle Enterprise Linux 6.7 (32-bit) 
-Red Hat Enterprise Linux 6.1, 6.2, 6.3, 6.4, 6.5, and 6.6 (32-bit and 64-bit)
-</t>
+Red Hat Enterprise Linux 6.1, 6.2, 6.3, 6.4, 6.5, and 6.6 (32-bit and 64-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">The Xen front-end NIC driver is defective. Resource leak occurs when a VM deletes the granted references.</t>
@@ -400,8 +431,8 @@
     <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/drivers/net/xen-netfront.c?id=cefe0078eea52af17411eb1248946a94afb84ca5</t>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, and 6.7 (32-bit and 64-bit) 
-CentOS 6.8 (64-bit) 
+    <t xml:space="preserve">CentOS 6.1, 6.2, 6.3, 6.4, 6.5, 6.6, 6.7, and 6.8 (32-bit and 64-bit) 
+Oracle Enterprise Linux 5.8 (64-bit)
 Red Hat Enterprise Linux 6.1, 6.2, 6.3, 6.4, 6.5 and 6.6 (32-bit and 64-bit)</t>
   </si>
   <si>
@@ -436,8 +467,14 @@
     <t xml:space="preserve">The actual memory size displayed to users is smaller than the configured one. </t>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 5.11 (32-bit and 64-bit) 
-Novell SuSE Linux Enterprise Server 11 SP1 and SP2 
+    <t xml:space="preserve">CentOS 5.4 (32-bit and 64-bit)
+CentOS 5.5 (32-bit and 64-bit)
+CentOS 5.11 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 11 SP1 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 11 SP2 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 11 SP3 (32-bit and 64-bit)
+Red Hat Enterprise Linux 5.4 (32-bit and 64-bit)
+Red Hat Enterprise Linux 5.5 (32-bit and 64-bit)
 Red Hat Enterprise Linux 5.11 (32-bit and 64-bit)</t>
   </si>
   <si>
@@ -455,7 +492,9 @@
 2. Restart the VM for the new configurations to take effect. </t>
   </si>
   <si>
-    <t xml:space="preserve">CentOS 5.11 (32-bit and 64-bit) 
+    <t xml:space="preserve">CentOS 5.5 (32-bit and 64-bit)
+CentOS 5.11 (32-bit and 64-bit)
+Red Hat Enterprise Linux 5.5 (32-bit and 64-bit)
 Red Hat Enterprise Linux 5.11 (32-bit and 64-bit)</t>
   </si>
   <si>
@@ -550,12 +589,13 @@
     <t xml:space="preserve">The VM does not respond when it is being restored using a snapshot. </t>
   </si>
   <si>
-    <t xml:space="preserve">Debian GNU and Linux 8.2.0 (32-bit and 64-bit) 
-Fedora 23 (64-bit) 
-Oracle Linux 7.2 (64-bit) 
-Ubuntu server 14.04.2 (32-bit and 64-bit) 
-Ubuntu server 14.04.3 (32-bit)
-</t>
+    <t xml:space="preserve">Debian GNU/Linux 8.0.0 (32-bit and 64-bit)
+Debian GNU/Linux 8.2.0 (32-bit and 64-bit)
+Fedora 23 (64-bit)
+Oracle Linux 7.2 (64-bit)
+Ubuntu Server 14.04.2 (32-bit and 64-bit)
+Ubuntu Server 14.04.3 (32-bit and 64-bit)
+Ubuntu Server 14.10 (32-bit and 64-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">The front-end NIC driver of a VM is defective: When you use the host to uninstall a down NIC from a VM or initiate hibernation, wake-up, live migration, or snapshot for a VM whose NIC is down, the front-end NIC driver of the VM calls the napi synchronization function. Executing this function causes the xenwatch thread to enter the D state. </t>
@@ -600,7 +640,7 @@
     <t xml:space="preserve">CoreOS 1010.5.0
 CoreOS 1068.2.0
 CoreOS 1122.2.0
-</t>
+CoreOS 1122.3.0</t>
   </si>
   <si>
     <t xml:space="preserve">The libxenstore component built in the VM is defective. The libxenstore.so library file of the VM accesses the /proc/xen/xenbus interface file by default. When the user-space program (for example, uvp-monitor process) registers the xenwatch through the libxenstore.so, the VM kernel reads and writes the Xenstore, which triggers a conflict with the RCU lock mechanism of the kernel process file system. </t>
@@ -719,7 +759,11 @@
     <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=7098296a362a96051fa120abf48f0095818b99cd</t>
   </si>
   <si>
-    <t xml:space="preserve">Ubuntu server 16.04 (64-bit)</t>
+    <t xml:space="preserve">Ubuntu Server 16.04 (32-bit and 64-bit)
+Ubuntu Server 16.04.1 (32-bit and 64-bit)
+Ubuntu Server/Desktop 14.04.4 (32-bit)
+Ubuntu Server 14.04.5 (64-bit)
+openSUSE Leap 42.2 (64-bit)</t>
   </si>
   <si>
     <t xml:space="preserve">The VM kernel has a defect. On a Xen virtualization platform, when the VM uses the qspinlocks, a CPU may try to kick another CPU that is spinning (because the spinning CPU has not initialized its kicker interrupt). However, due to this defect, a CPU may kick another CPU that has not completed the interrupt allocation during VM startup. As a result, the VM crashes, and the VNC encounters a black screen error.</t>
@@ -744,7 +788,8 @@
   </si>
   <si>
     <t xml:space="preserve">CoreOS 1122.2.0
-CoreOS 1122.3.0</t>
+CoreOS 1122.3.0
+CoreOS 1185.5.0</t>
   </si>
   <si>
     <t xml:space="preserve">A defect is introduced to the xenbus module during the modification of the VM kernel. Due to this defect, user-space programs of VMs running on Xen fail to access the Xenstore, and the uvp-monitor process fails to run as well. 
@@ -757,6 +802,299 @@
   </si>
   <si>
     <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/drivers/xen/xenbus/xenbus_dev_frontend.c?h=linux-4.7.y&amp;id=b035f15daf750e1594964d68889e0de5c3014922</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubuntu 16.04 (32-bit) (kernel version: 4.4.0-21-generic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. xen_pfn_to_page is introduced to Linux kernel 4.4-rc1 in the Linux Kernel community. When conversion between pfns and pages is performed on a Xen VM, if the VM memory reaches 4 GB, pfn overflow will occur during conversion. As a result, the VM crashes during startup.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a VM is configured with 4 GB or more memory, the VM will crash during startup. (Sometimes, this problem will also occur if large pfn values are used to manage memory of a VM configured with more than 3 GB of memory.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=60901df3aed230d4565dca003f11b6a95fbf30d9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suggestion 1:
+This patch has been incorporated into Linux kernel 4.6-rc7 in the Linux Kernel community. Refer to the link for method to fix this bug.
+Suggestion 2:
+Do not configure a 32-bit OS with more than 3 GB of memory.
+Suggestion 3:
+Upgrade the OS to Ubuntu 16.04.1 or a later distribution.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 11 SP1 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.3 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective.
+When finding the busiest task group, the system calculates the average load of each task by dividing the total load by the number of currently running queues (rq-&gt; nr_running). But rq-&gt; nr_running is refreshed in each tick, that is, the number of running queues may be cleared during clock interrupt period. In this case, the "division by zero" error occurs and the VM stops responding.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMs occasionally stop responding during running because the task scheduling module is defective.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=4cd4262034849da01eb88659af677b69f8169f06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fedora 24 (64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During VM migration, the system needs to obtain interrupt lock resources, but the disabled interrupt lock resources have been released. As a result, the kernel function irq_move_masked_irq is locked out, the CPU usage is 100%, and the CPU is crashed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After live migration, VMs may stop responding.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=f0f393877c71ad227d36705d61d1e4062bc29cf5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubuntu Server 16.04 (32-bit)
+Ubuntu Server 16.04 (64-bit)
+Ubuntu Server 16.04.1 (32-bit)
+Ubuntu Server 16.04.1 (64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Xen balloon driver that comes with the VM (configured with less than eight vCPUs and 8 GB of memory) kernel is defective. The Xen balloon driver supports memory hot plug. If the memory size (current_pages) that the Xen balloon driver obtains through the get_num_physpages interface is smaller than the memory size (target_pages) that the CNA node assigns to it, the Xen balloon driver automatically executes the memory hot-plug process even thought the hypervisor does not deliver the memory hot-plug command to the VM, to add the memory difference (target_pages – current_pages) to the VM. Actually, no memory is hot-plugged into the VM. The memory added to the VM is the IO system memory (memory that the kernel reserves for the IO system). However, the cache that the CD-ROM drive has obtained happens to contain the memory added to the VM. As a result, some files read from the CD-ROM drive of the VM are abnormal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a VM is configured with less than eight vCPUs and 8 GB of memory, some files read from the CD-ROM drive of the VM are abnormal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/drivers/xen/balloon.c?id=782b86641e5d471e9eb1cf0072c012d2f758e568
+https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/include/linux/ioport.h?id=9babd5c8caa6e62c116efc3a64a09f65af4112b0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.3 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.3 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VM kernels are not compatible with the virtualization platform. Repeatedly hot swapping VM disks or hibernating VMs occasionally makes the VM TSC clock source unstable. The xenwatch_unplug thread running timeout blocks the xenwatch thread. As a result, VM hibernation fails.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After VM disks or NICs are hot swapped repeatedly, the live migration or hibernation of VMs may fail.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the clock source in the VM.
+In the /boot/grub/menu.lst file of VMs, add the notsc or tsc=reliable parameter to the default boot options. For example, kernel /vmlinuz-2.6.32-279.el6.x86_64 ro root=/dev/mapper/vg-localhost-lv_root notsc. The default boot options are the value of default in /boot/grub/menu.lst.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.1 (32-bit and 64-bit)
+CentOS 6.2 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.1 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.2 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The front-end disk driver of the VM is defective. When the disk is hot-plugged out from a VM, if blk_cleanup_queue() is called before the call to del_gendisk() and the memory allocated to request_queue is released, the uevent that is occasionally sent by del_gendisk() to read the memory allocated to request_queue will read invalid memory. As a result, a kernel panic occurs on the VM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a disk is hot-plugged out from a VM, a kernel panic occurs on the VM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/drivers/block/xen-blkfront.c?id=89de1669ace055b56f1de1c9f5aca26dd7f17f25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 6.7 (32-bit and 64-bit)
+Debian GNU/Linux 8.2.0 (32-bit and 64-bit)
+Debian GNU/Linux 8.6.0 (32-bit and 64-bit)
+Debian GNU/Linux 8.7.0 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 12 SP1 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 12 SP2 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During VM login through a serial port, if you continuously input data through the serial port, a kernel panic occasionally occurs when alarm information is returned. As a result, the VM fails to start up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMs occasionally fail to start up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restart VMs or avoid inputting data to VMs through the serial port during VM startup.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubuntu Server 14.04 (32-bit)
+Ubuntu Server 14.04 (64-bit)
+Ubuntu Server 16.04 (32-bit)
+Ubuntu Server 16.04 (64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. During VM migration, the system needs to obtain interrupt lock resources, but the disabled interrupt lock resources have been released. As a result, the kernel function irq_move_masked_irq is locked out, the CPU usage is 100%, and the CPU is crashed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The live migration, snapshot, or hibernation of VMs fails occasionally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/?id=ff1e22e7a638a0782f54f81a6c9cb139aca2da35
+https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/?id=f0f393877c71ad227d36705d61d1e4062bc29cf5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 11 SP1 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective.
+If vCPUs go online in parallel mode, vCPU A holds the read lock of an interrupt request, vCPU B runs set_mtrr and integrates MTRR using IPI, and vCPU C disables IRQs using write_lock_irq, vCPU C will be in the deadlock status and fail to go online, and its kernel thread fails to run and in the uninterruptible sleep status.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After vCPUs go online in parallel mode, some processes of the VM OS are occasionally in the uninterruptible sleep status.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/arch/x86/kernel/smpboot.c?id=68f202e4e87cfab4439568bf397fcc5c7cf8d729</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install the corrective patch or make vCPUs online in serial mode.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 11 SP3 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The libata driver in the VM kernel is defective.
+hsm_task_stat supports concurrent access. Due to lack of lock protection, kernel panics may occur under high I/O pressure. For details, see the kernel BUG at /usr/src/packages/BUILD/kernel-default-3.0.76/linux-3.0/drivers/ata/libata-sff.c:1298! field in the core file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the libata driver is enabled, kernel panics may occur when the disk pressure is increasing or the I/O pressure on back-end disks is high.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/drivers/ata/libata-sff.c?id=ce7514526742c0898b837d4395f515b79dfb5a12
+https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/drivers/ata/libata-sff.c?id=a588afc920bc50e894f6ae2874c4281c795e0979
+https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/drivers/ata/libata-sff.c?id=8eee1d3ed5b6fc8e14389567c9a6f53f82bb7224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canaima GNU/Linux 3.1 (32-bit and 64-bit)
+Debian GNU/Linux 6.0.4 (64-bit)
+Debian GNU/Linux 6.0.5 (64-bit)
+Debian GNU/Linux 6.0.7 (64-bit)
+Debian GNU/Linux 6.0.10 (64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective. If a VM is configured with more than six vCPUs, the VM stops responding during its startup.
+The system registers clock interrupt for each vCPU. The clock interrupt number starts from 16, closely followed by the xenbus interrupt number. If the number of vCPUs is larger than 6, No. 23 (the fix interrupt number of the PCI device UHCI) is occupied. As a result, UHCI interrupt registration fails, vCPUs cannot be scheduled, and the VM cannot be started.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If a VM is configured with more than six vCPUs, the VM cannot be started.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configure no more than six vCPUs on a VM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Novell SuSE Linux Enterprise Server 11 SP1 (32-bit)
+openSUSE Leap 42.1 (64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective.
+By default, when an NIC is configured for a VM, a simulated device (RTL 8139 NIC) and the Xen paravirtual front-end NIC appear and coexist in the VM. During the initialization of the VM kernel, the kernel asks the hypervisor to destroy the simulated device. Then live migration is performed for the first time and is successful. However, due to the defective live migration process, the simulated device is not destroyed during the VM restoration phase of the live migration process. Therefore, after live migration, the simulated device can still be detected in the VM. The NIC configured for the VM is now hot-plugged out, the VM, however, cannot reclaim the memory allocated to the NIC due to kernel defect. Then live migration of the VM is performed again. After the VM is moved to the destination, the VM attempts to restore the simulated device, during which time memory access will be abnormal. As a result, the VM crashes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If an NIC is hot-plugged out from a VM after live migration and then live migration is performed again, the VM will crash.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To restore the VM after the problem occurs, forcibly restart the VM.
+Suggestion:
+Do not hot-plug out NICs after live migration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ubuntu Server 16.04.1 (32-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The xen-balloon driver of the VM kernel is defective. After the OS is booted, the balloon driver triggers a memory hot swap, which re-maps the memory used by the I/O address space and adds the memory address to linear addresses. In this case, one physical page is mapped to two linear addresses. If a kernel stack is located in such physical page, the stack may be modified by other threads. As a result, the stack becomes abnormal, and the VM crashes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM occasionally crashes during startup or running.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Install the corrective patch to fix this bug.
+To immediately restore the VM, forcibly restart the VM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Red Hat Enterprise Linux 5.4 (64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The IPv6 module in the VM kernel is defective. A null pointer reference vulnerability exists in the kernel function ip6_dst_lookup_tail. Attackers on the local network can exploit this vulnerability by sending IPv6 packets to the targeted system. If dst-&gt;neighbour on the system is null, the system will be crashed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMs are occasionally crashed during running.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://rhn.redhat.com/errata/RHSA-2010-0147.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method 1:
+Disable IPv6.
+1.    Add the following information to the /etc/modprobe.conf file:
+alias net-pf-10 off alias ipv6 off
+2.    In the /etc/sysconfig/network file, confirm the following setting: NETWORKING_IPV6=no.
+3.    Restart the VM.
+Method 2:
+Install the Red Hat official corrective patch.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 5.5 (32-bit and 64-bit)
+Red Hat Enterprise Linux 5.5 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective.
+On the host which is installed with AMD Opteron 6000 series CPUs, kernel panics occur and VMs fail to be started.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VMs fail to be started.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://access.redhat.com/site/articles/37935</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l  Install the corrective patch.
+l  Upgrade the OS to CentOS 5.6 or later.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CentOS 5 (32-bit and 64-bit)
+Red Hat Enterprise Linux 5 (32-bit and 64-bit)
+Oracle 5 (32-bit and 64-bit)
+Novell SuSE Linux Enterprise Server 11 SP1 (32-bit and 64-bit)
+Oracle Linux Server release 6.3 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.0 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.1 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.2 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.3 (32-bit and 64-bit)
+Red Hat Enterprise Linux 6.4 (32-bit and 64-bit)
+CentOS 6.0 (32-bit and 64-bit)
+CentOS 6.1 (32-bit and 64-bit)
+CentOS 6.2 (32-bit and 64-bit)
+CentOS 6.3 (32-bit and 64-bit)
+CentOS 6.4 (32-bit and 64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective.
+When guestNuma is enabled in the VM and the VM is configured with a specific CPU topology, the incorrect calculation that the VM kernel performs on the mapping between memory and the nodes associated with CPUs results in a divide-by-zero bug. As a result, a kernel panic occurs on the VM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM fails to be started.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/pub/scm/linux/kernel/git/torvalds/linux.git/commit/?id=7d6b46707f2491a94f4bd3b4329d2d7f809e9368</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective.
+When a device is registered with sysfs, if the group attributes of the device are not set, the grp-&gt;attrs variable is null. When sysfs creates the group to which the device belongs, sysfs directly uses the grp-&gt;attrs variable without checking it. As a result, a null pointer is accessed, and the VM crashes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://git.kernel.org/pub/scm/linux/kernel/git/torvalds/linux.git/commit/?id=5631f2c18f4b2845b3e97df1c659c5094a17605f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openSUSE Leap 42.2 (64-bit)
+Novell SuSE Linux Enterprise Server 12 SP2 (64-bit)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM kernel is defective.
+During the VM restoration phase of live migration and hibernation wakeup, child devices restored synchronously are dependent on the parent device (the child devices and the parent device are restored asynchronously). When the parent device has not been restored, the child devices are holding the lock and keep waiting for the parent device to recover. The parent device cannot obtain the lock and therefore cannot be restored. This will result in a deadlock.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The VM occasionally crashes during live migration and wakeup.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To restore the VM after the problem occurs, forcibly restart the VM.
+To avoid this problem, modify the kernel code. Add "pm_async_enable = 0" in the dpm_resume_noirq function to disable asynchronous restoration.</t>
   </si>
 </sst>
 </file>
@@ -1205,10 +1543,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1350,7 +1688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="117" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="17" t="s">
         <v>25</v>
       </c>
@@ -1361,7 +1699,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="17" t="s">
         <v>28</v>
       </c>
@@ -1372,7 +1710,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="17" t="s">
         <v>31</v>
       </c>
@@ -1381,6 +1719,17 @@
       </c>
       <c r="C21" s="18" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1412,10 +1761,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1454,39 +1803,39 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1494,19 +1843,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,19 +1863,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,59 +1883,59 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="236.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="332.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="116.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E8" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>66</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="157.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,19 +1943,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,39 +1963,39 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="116.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,19 +2003,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1674,19 +2023,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="173.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,19 +2043,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1714,39 +2063,39 @@
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1754,19 +2103,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1774,19 +2123,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,39 +2143,39 @@
         <v>18</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="154.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="47.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1834,19 +2183,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1854,19 +2203,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,59 +2223,59 @@
         <v>22</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="283.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="218.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="24" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F24" s="23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="24" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F25" s="23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,39 +2283,39 @@
         <v>25</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="189" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="160.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="24" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,39 +2323,39 @@
         <v>27</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="110.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="24" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="126" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,19 +2363,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,19 +2383,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="103.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2054,19 +2403,19 @@
         <v>31</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="123" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2074,19 +2423,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2094,19 +2443,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2114,19 +2463,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="191.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2134,19 +2483,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="139.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2154,19 +2503,19 @@
         <v>36</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="94.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2174,39 +2523,399 @@
         <v>37</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="157.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="122.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="24" t="n">
         <v>38</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="24" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="24" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="24" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="192.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="24" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="65.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="24" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="24" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="24" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="65.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="24" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="24" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="24" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="D49" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="E49" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="24" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="D50" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="205.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="24" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C51" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="D51" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="90.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="24" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="D52" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="24" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="C53" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="E53" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="24" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="F54" s="23" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="205.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="24" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="E55" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="77.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="24" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="E56" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="F56" s="23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="103.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="24" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="E57" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="F57" s="23" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2226,6 +2935,15 @@
     <hyperlink ref="E31" r:id="rId13" display="https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/arch/x86/xen/smp.c?id=184748cc50b2dceb8287f9fb657eda48ff8fcfe7"/>
     <hyperlink ref="E36" r:id="rId14" display="https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=7098296a362a96051fa120abf48f0095818b99cd"/>
     <hyperlink ref="E37" r:id="rId15" display="https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=707e59ba494372a90d245f18b0c78982caa88e48"/>
+    <hyperlink ref="E40" r:id="rId16" display="https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=60901df3aed230d4565dca003f11b6a95fbf30d9"/>
+    <hyperlink ref="E41" r:id="rId17" display="https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=4cd4262034849da01eb88659af677b69f8169f06"/>
+    <hyperlink ref="E42" r:id="rId18" display="https://git.kernel.org/cgit/linux/kernel/git/torvalds/linux.git/commit/?id=f0f393877c71ad227d36705d61d1e4062bc29cf5"/>
+    <hyperlink ref="E45" r:id="rId19" display="https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/drivers/block/xen-blkfront.c?id=89de1669ace055b56f1de1c9f5aca26dd7f17f25"/>
+    <hyperlink ref="E48" r:id="rId20" display="https://git.kernel.org/cgit/linux/kernel/git/stable/linux-stable.git/commit/arch/x86/kernel/smpboot.c?id=68f202e4e87cfab4439568bf397fcc5c7cf8d729"/>
+    <hyperlink ref="E53" r:id="rId21" display="https://rhn.redhat.com/errata/RHSA-2010-0147.html"/>
+    <hyperlink ref="E54" r:id="rId22" display="https://access.redhat.com/site/articles/37935"/>
+    <hyperlink ref="E55" r:id="rId23" display="https://git.kernel.org/pub/scm/linux/kernel/git/torvalds/linux.git/commit/?id=7d6b46707f2491a94f4bd3b4329d2d7f809e9368"/>
+    <hyperlink ref="E56" r:id="rId24" display="https://git.kernel.org/pub/scm/linux/kernel/git/torvalds/linux.git/commit/?id=5631f2c18f4b2845b3e97df1c659c5094a17605f"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>